<commit_message>
Updated tyranids and guard
</commit_message>
<xml_diff>
--- a/Raw Data/weapons.xlsx
+++ b/Raw Data/weapons.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Battlescribe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahoan\Documents\github\40kLite\40klite\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D9735F-6AE5-415A-9D86-E1541BBB4AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4F64CE-6B07-4E93-A2B5-D63D964E425A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="0" windowWidth="16515" windowHeight="17145" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>Weapon</t>
   </si>
@@ -213,6 +213,30 @@
   </si>
   <si>
     <t>Basilisk Earthshaker</t>
+  </si>
+  <si>
+    <t>Manticore</t>
+  </si>
+  <si>
+    <t>No sponsons</t>
+  </si>
+  <si>
+    <t>good mele</t>
+  </si>
+  <si>
+    <t>Rupture Cannon</t>
+  </si>
+  <si>
+    <t>Fleshborer Hive</t>
+  </si>
+  <si>
+    <t>Acid Spray</t>
+  </si>
+  <si>
+    <t>Impaler</t>
+  </si>
+  <si>
+    <t>Shock</t>
   </si>
 </sst>
 </file>
@@ -647,10 +671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFAFC17-B8CC-4FDE-905B-FC2D8F8BC7C4}">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,10 +1039,10 @@
         <v>-1</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <f t="shared" si="8"/>
@@ -1026,11 +1050,11 @@
       </c>
       <c r="I13">
         <f t="shared" si="4"/>
-        <v>0.3888888888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
-        <v>0.33333333333333331</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="K13">
         <f t="shared" si="6"/>
@@ -1089,10 +1113,10 @@
         <v>-1</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15">
         <f t="shared" si="8"/>
@@ -1100,407 +1124,416 @@
       </c>
       <c r="I15">
         <f t="shared" si="4"/>
-        <v>0.44444444444444442</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J15">
         <f t="shared" si="5"/>
-        <v>0.27777777777777779</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K15">
         <f t="shared" si="6"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D18" si="9">(24-C16)/12</f>
+        <v>-2</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <f>SUM(D16:F16)/B16</f>
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16">
+        <f>(2/3)*$B16*((13-E16)/12)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="J16">
+        <f>(2/3)*$B16*((13-F16)/12)</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K16:K18" si="10">I16+J16</f>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D17">
-        <f>(24-C17)/12</f>
-        <v>-1</v>
+        <f t="shared" si="9"/>
+        <v>-4</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G17">
         <f>SUM(D17:F17)/B17</f>
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
       </c>
       <c r="I17">
         <f>(2/3)*$B17*((13-E17)/12)</f>
-        <v>0.27777777777777779</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J17">
         <f>(2/3)*$B17*((13-F17)/12)</f>
-        <v>0.16666666666666666</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="K17">
-        <f>I17+J17</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="10"/>
+        <v>0.83333333333333326</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="D18">
-        <f>(24-C18)/12</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>-4</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G18">
         <f>SUM(D18:F18)/B18</f>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="I18">
         <f>(2/3)*$B18*((13-E18)/12)</f>
-        <v>0.33333333333333331</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J18">
         <f>(2/3)*$B18*((13-F18)/12)</f>
-        <v>0.16666666666666666</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="K18">
-        <f>I18+J18</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I19">
-        <f>(2/3)*$B19*((13-E19)/12)</f>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <f>(2/3)*$B19*((13-F19)/12)</f>
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <f>I19+J19</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>0.83333333333333326</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <f>(24-C20)/12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F20">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20">
         <f>SUM(D20:F20)/B20</f>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="I20">
-        <f>(2/3)*$B20*((13-E20)/12)</f>
-        <v>1</v>
+        <f t="shared" ref="I20:I31" si="11">(2/3)*$B20*((13-E20)/12)</f>
+        <v>0.27777777777777779</v>
       </c>
       <c r="J20">
-        <f>(2/3)*$B20*((13-F20)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" ref="J20:J31" si="12">(2/3)*$B20*((13-F20)/12)</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K20">
-        <f>I20+J20</f>
-        <v>1.3333333333333333</v>
+        <f t="shared" ref="K20:K31" si="13">I20+J20</f>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D21">
         <f>(24-C21)/12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G21">
         <f>SUM(D21:F21)/B21</f>
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
       </c>
       <c r="I21">
-        <f>(2/3)*$B21*((13-E21)/12)</f>
-        <v>0.88888888888888884</v>
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J21">
-        <f>(2/3)*$B21*((13-F21)/12)</f>
-        <v>0.55555555555555558</v>
+        <f t="shared" si="12"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K21">
-        <f>I21+J21</f>
-        <v>1.4444444444444444</v>
+        <f t="shared" si="13"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>24</v>
-      </c>
-      <c r="D22">
-        <f>(24-C22)/12</f>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>8</v>
-      </c>
-      <c r="F22">
-        <v>6</v>
-      </c>
-      <c r="G22">
-        <f>SUM(D22:F22)/B22</f>
-        <v>7</v>
-      </c>
       <c r="I22">
-        <f>(2/3)*$B22*((13-E22)/12)</f>
-        <v>0.55555555555555558</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="J22">
-        <f>(2/3)*$B22*((13-F22)/12)</f>
-        <v>0.77777777777777779</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="K22">
-        <f>I22+J22</f>
-        <v>1.3333333333333335</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D23">
-        <f>(24-C23)/12</f>
-        <v>1</v>
+        <f t="shared" ref="D23:D31" si="14">(24-C23)/12</f>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F23">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G23">
-        <f>SUM(D23:F23)/B23</f>
-        <v>14</v>
+        <f t="shared" ref="G23:G31" si="15">SUM(D23:F23)/B23</f>
+        <v>6</v>
       </c>
       <c r="I23">
-        <f>(2/3)*$B23*((13-E23)/12)</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="11"/>
+        <v>1</v>
       </c>
       <c r="J23">
-        <f>(2/3)*$B23*((13-F23)/12)</f>
-        <v>0.27777777777777779</v>
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K23">
-        <f>I23+J23</f>
-        <v>0.72222222222222221</v>
+        <f t="shared" si="13"/>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D24">
-        <f>(24-C24)/12</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>5</v>
       </c>
       <c r="F24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <f>SUM(D24:F24)/B24</f>
-        <v>14</v>
+        <f t="shared" si="15"/>
+        <v>7</v>
       </c>
       <c r="I24">
-        <f>(2/3)*$B24*((13-E24)/12)</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="11"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J24">
-        <f>(2/3)*$B24*((13-F24)/12)</f>
-        <v>0.22222222222222221</v>
+        <f t="shared" si="12"/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="K24">
-        <f>I24+J24</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="13"/>
+        <v>1.4444444444444444</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25">
-        <f>(24-C25)/12</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <f>SUM(D25:F25)/B25</f>
-        <v>14</v>
+        <f t="shared" si="15"/>
+        <v>7</v>
       </c>
       <c r="I25">
-        <f>(2/3)*$B25*((13-E25)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="11"/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="J25">
-        <f>(2/3)*$B25*((13-F25)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="12"/>
+        <v>0.77777777777777779</v>
       </c>
       <c r="K25">
-        <f>I25+J25</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="13"/>
+        <v>1.3333333333333335</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D26">
-        <f>(24-C26)/12</f>
-        <v>-1</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G26">
-        <f>SUM(D26:F26)/B26</f>
-        <v>8</v>
+        <f t="shared" si="15"/>
+        <v>14</v>
       </c>
       <c r="I26">
-        <f>(2/3)*$B26*((13-E26)/12)</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="11"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J26">
-        <f>(2/3)*$B26*((13-F26)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="12"/>
+        <v>0.27777777777777779</v>
       </c>
       <c r="K26">
-        <f>I26+J26</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="D27">
-        <f>(24-C27)/12</f>
-        <v>-4</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G27">
-        <f>SUM(D27:F27)/B27</f>
-        <v>6.5</v>
+        <f t="shared" si="15"/>
+        <v>14</v>
       </c>
       <c r="I27">
-        <f>(2/3)*$B27*((13-E27)/12)</f>
+        <f t="shared" si="11"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="12"/>
         <v>0.22222222222222221</v>
       </c>
-      <c r="J27">
-        <f>(2/3)*$B27*((13-F27)/12)</f>
-        <v>0.77777777777777779</v>
-      </c>
       <c r="K27">
-        <f>I27+J27</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1509,72 +1542,109 @@
         <v>24</v>
       </c>
       <c r="D28">
-        <f>(24-C28)/12</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E28">
         <v>7</v>
       </c>
       <c r="F28">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="13"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="14"/>
+        <v>-1</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
         <v>10</v>
       </c>
-      <c r="G28">
-        <f>SUM(D28:F28)/B28</f>
-        <v>17</v>
-      </c>
-      <c r="I28">
-        <f>(2/3)*$B28*((13-E28)/12)</f>
+      <c r="G29">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="11"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J28">
-        <f>(2/3)*$B28*((13-F28)/12)</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K28">
-        <f>I28+J28</f>
-        <v>0.5</v>
+      <c r="K29">
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D30">
-        <f>(24-C30)/12</f>
-        <v>-1</v>
+        <f t="shared" si="14"/>
+        <v>-4</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G30">
-        <f>SUM(D30:F30)/B30</f>
-        <v>14</v>
+        <f t="shared" si="15"/>
+        <v>6.5</v>
       </c>
       <c r="I30">
-        <f>(2/3)*$B30*((13-E30)/12)</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="11"/>
+        <v>0.22222222222222221</v>
       </c>
       <c r="J30">
-        <f>(2/3)*$B30*((13-F30)/12)</f>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="12"/>
+        <v>0.77777777777777779</v>
       </c>
       <c r="K30">
-        <f>I30+J30</f>
-        <v>0.61111111111111105</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1583,72 +1653,35 @@
         <v>24</v>
       </c>
       <c r="D31">
-        <f>(24-C31)/12</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G31">
-        <f>SUM(D31:F31)/B31</f>
-        <v>13</v>
+        <f t="shared" si="15"/>
+        <v>17</v>
       </c>
       <c r="I31">
-        <f>(2/3)*$B31*((13-E31)/12)</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J31">
-        <f>(2/3)*$B31*((13-F31)/12)</f>
-        <v>0.27777777777777779</v>
+        <f t="shared" si="12"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K31">
-        <f>I31+J31</f>
-        <v>0.72222222222222221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>36</v>
-      </c>
-      <c r="D32">
-        <f>(24-C32)/12</f>
-        <v>-1</v>
-      </c>
-      <c r="E32">
-        <v>7</v>
-      </c>
-      <c r="F32">
-        <v>7</v>
-      </c>
-      <c r="G32">
-        <f>SUM(D32:F32)/B32</f>
-        <v>13</v>
-      </c>
-      <c r="I32">
-        <f>(2/3)*$B32*((13-E32)/12)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="J32">
-        <f>(2/3)*$B32*((13-F32)/12)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K32">
-        <f>I32+J32</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="13"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1657,127 +1690,146 @@
         <v>36</v>
       </c>
       <c r="D33">
-        <f>(24-C33)/12</f>
+        <f t="shared" ref="D33:D38" si="16">(24-C33)/12</f>
         <v>-1</v>
       </c>
       <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
         <v>10</v>
       </c>
-      <c r="F33">
-        <v>4</v>
-      </c>
       <c r="G33">
-        <f>SUM(D33:F33)/B33</f>
-        <v>13</v>
+        <f t="shared" ref="G33:G48" si="17">SUM(D33:F33)/B33</f>
+        <v>14</v>
       </c>
       <c r="I33">
-        <f>(2/3)*$B33*((13-E33)/12)</f>
+        <f t="shared" ref="I33:I48" si="18">(2/3)*$B33*((13-E33)/12)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J33">
+        <f t="shared" ref="J33:J48" si="19">(2/3)*$B33*((13-F33)/12)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="J33">
-        <f>(2/3)*$B33*((13-F33)/12)</f>
-        <v>0.5</v>
-      </c>
       <c r="K33">
-        <f>I33+J33</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" ref="K33:K48" si="20">I33+J33</f>
+        <v>0.61111111111111105</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D34">
-        <f>(24-C34)/12</f>
-        <v>-2</v>
+        <f t="shared" si="16"/>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F34">
         <v>8</v>
       </c>
       <c r="G34">
-        <f>SUM(D34:F34)/B34</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="I34">
-        <f>(2/3)*$B34*((13-E34)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="18"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J34">
-        <f>(2/3)*$B34*((13-F34)/12)</f>
+        <f t="shared" si="19"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K34">
-        <f>I34+J34</f>
-        <v>0.61111111111111116</v>
+        <f t="shared" si="20"/>
+        <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D35">
-        <f>(24-C35)/12</f>
-        <v>1</v>
+        <f t="shared" si="16"/>
+        <v>-1</v>
       </c>
       <c r="E35">
         <v>7</v>
       </c>
       <c r="F35">
+        <v>7</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="18"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="19"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="20"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>36</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="E36">
         <v>10</v>
       </c>
-      <c r="G35">
-        <f>SUM(D35:F35)/B35</f>
-        <v>9</v>
-      </c>
-      <c r="I35">
-        <f>(2/3)*$B35*((13-E35)/12)</f>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="18"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="19"/>
+        <v>0.5</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="20"/>
         <v>0.66666666666666663</v>
-      </c>
-      <c r="J35">
-        <f>(2/3)*$B35*((13-F35)/12)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K35">
-        <f>I35+J35</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G36" t="e">
-        <f>SUM(D36:F36)/B36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I36">
-        <f>(2/3)*$B36*((13-E36)/12)</f>
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <f>(2/3)*$B36*((13-F36)/12)</f>
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <f>I36+J36</f>
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1786,7 +1838,7 @@
         <v>48</v>
       </c>
       <c r="D37">
-        <f>(24-C37)/12</f>
+        <f t="shared" si="16"/>
         <v>-2</v>
       </c>
       <c r="E37">
@@ -1796,99 +1848,80 @@
         <v>8</v>
       </c>
       <c r="G37">
-        <f>SUM(D37:F37)/B37</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="I37">
-        <f>(2/3)*$B37*((13-E37)/12)</f>
+        <f t="shared" si="18"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J37">
-        <f>(2/3)*$B37*((13-F37)/12)</f>
+        <f t="shared" si="19"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K37">
-        <f>I37+J37</f>
+        <f t="shared" si="20"/>
         <v>0.61111111111111116</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D38">
-        <f>(24-C38)/12</f>
-        <v>-1</v>
+        <f t="shared" si="16"/>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="G38">
-        <f>SUM(D38:F38)/B38</f>
-        <v>13</v>
-      </c>
       <c r="I38">
-        <f>(2/3)*$B38*((13-E38)/12)</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="18"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J38">
-        <f>(2/3)*$B38*((13-F38)/12)</f>
-        <v>0.22222222222222221</v>
+        <f t="shared" si="19"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K38">
-        <f>I38+J38</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="20"/>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>24</v>
-      </c>
-      <c r="D39">
-        <f>(24-C39)/12</f>
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>6</v>
-      </c>
-      <c r="F39">
-        <v>7</v>
-      </c>
-      <c r="G39">
-        <f>SUM(D39:F39)/B39</f>
-        <v>13</v>
+      <c r="G39" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="I39">
-        <f>(2/3)*$B39*((13-E39)/12)</f>
-        <v>0.3888888888888889</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="J39">
-        <f>(2/3)*$B39*((13-F39)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
       <c r="K39">
-        <f>I39+J39</f>
-        <v>0.72222222222222221</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1897,7 +1930,7 @@
         <v>48</v>
       </c>
       <c r="D40">
-        <f>(24-C40)/12</f>
+        <f t="shared" ref="D40:D48" si="21">(24-C40)/12</f>
         <v>-2</v>
       </c>
       <c r="E40">
@@ -1907,62 +1940,62 @@
         <v>8</v>
       </c>
       <c r="G40">
-        <f>SUM(D40:F40)/B40</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="I40">
-        <f>(2/3)*$B40*((13-E40)/12)</f>
+        <f t="shared" si="18"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J40">
-        <f>(2/3)*$B40*((13-F40)/12)</f>
+        <f t="shared" si="19"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K40">
-        <f>I40+J40</f>
+        <f t="shared" si="20"/>
         <v>0.61111111111111116</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D41">
-        <f>(24-C41)/12</f>
-        <v>-2</v>
+        <f t="shared" si="21"/>
+        <v>-1</v>
       </c>
       <c r="E41">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F41">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <f>SUM(D41:F41)/B41</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="I41">
-        <f>(2/3)*$B41*((13-E41)/12)</f>
-        <v>0.27777777777777779</v>
+        <f t="shared" si="18"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J41">
-        <f>(2/3)*$B41*((13-F41)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="19"/>
+        <v>0.22222222222222221</v>
       </c>
       <c r="K41">
-        <f>I41+J41</f>
-        <v>0.61111111111111116</v>
+        <f t="shared" si="20"/>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1971,72 +2004,72 @@
         <v>24</v>
       </c>
       <c r="D42">
-        <f>(24-C42)/12</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="E42">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G42">
-        <f>SUM(D42:F42)/B42</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="I42">
-        <f>(2/3)*$B42*((13-E42)/12)</f>
-        <v>0.22222222222222221</v>
+        <f t="shared" si="18"/>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J42">
-        <f>(2/3)*$B42*((13-F42)/12)</f>
-        <v>0.5</v>
+        <f t="shared" si="19"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K42">
-        <f>I42+J42</f>
+        <f t="shared" si="20"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D43">
-        <f>(24-C43)/12</f>
-        <v>-1</v>
+        <f t="shared" si="21"/>
+        <v>-2</v>
       </c>
       <c r="E43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F43">
         <v>8</v>
       </c>
       <c r="G43">
-        <f>SUM(D43:F43)/B43</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="I43">
-        <f>(2/3)*$B43*((13-E43)/12)</f>
-        <v>0.3888888888888889</v>
+        <f t="shared" si="18"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J43">
-        <f>(2/3)*$B43*((13-F43)/12)</f>
+        <f t="shared" si="19"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K43">
-        <f>I43+J43</f>
-        <v>0.66666666666666674</v>
+        <f t="shared" si="20"/>
+        <v>0.61111111111111116</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2045,374 +2078,408 @@
         <v>48</v>
       </c>
       <c r="D44">
-        <f>(24-C44)/12</f>
+        <f t="shared" si="21"/>
         <v>-2</v>
       </c>
       <c r="E44">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G44">
-        <f>SUM(D44:F44)/B44</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="I44">
-        <f>(2/3)*$B44*((13-E44)/12)</f>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="18"/>
+        <v>0.27777777777777779</v>
       </c>
       <c r="J44">
-        <f>(2/3)*$B44*((13-F44)/12)</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="19"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K44">
-        <f>I44+J44</f>
-        <v>0.61111111111111105</v>
+        <f t="shared" si="20"/>
+        <v>0.61111111111111116</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D45">
-        <f>(24-C45)/12</f>
-        <v>1</v>
+        <f t="shared" si="21"/>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="18"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="19"/>
+        <v>0.5</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="20"/>
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>36</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="21"/>
+        <v>-1</v>
+      </c>
+      <c r="E46">
+        <v>6</v>
+      </c>
+      <c r="F46">
         <v>8</v>
       </c>
-      <c r="G45">
-        <f>SUM(D45:F45)/B45</f>
-        <v>14</v>
-      </c>
-      <c r="H45" t="s">
-        <v>22</v>
-      </c>
-      <c r="I45">
-        <f>(2/3)*$B45*((13-E45)/12)</f>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="J45">
-        <f>(2/3)*$B45*((13-F45)/12)</f>
+      <c r="G46">
+        <f t="shared" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="18"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="19"/>
         <v>0.27777777777777779</v>
       </c>
-      <c r="K45">
-        <f>I45+J45</f>
-        <v>0.72222222222222221</v>
+      <c r="K46">
+        <f t="shared" si="20"/>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47">
         <v>48</v>
       </c>
       <c r="D47">
-        <f>(24-C47)/12</f>
+        <f t="shared" si="21"/>
         <v>-2</v>
       </c>
       <c r="E47">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F47">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G47">
-        <f>SUM(D47:F47)/B47</f>
-        <v>6.5</v>
+        <f t="shared" si="17"/>
+        <v>13</v>
       </c>
       <c r="I47">
-        <f>(2/3)*$B47*((13-E47)/12)</f>
-        <v>0.55555555555555558</v>
+        <f t="shared" si="18"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="J47">
-        <f>(2/3)*$B47*((13-F47)/12)</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="19"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="K47">
-        <f>I47+J47</f>
-        <v>1.2222222222222223</v>
+        <f t="shared" si="20"/>
+        <v>0.61111111111111105</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D48">
-        <f>(24-C48)/12</f>
-        <v>-2</v>
+        <f t="shared" si="21"/>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F48">
         <v>8</v>
       </c>
       <c r="G48">
-        <f>SUM(D48:F48)/B48</f>
-        <v>13</v>
+        <f t="shared" si="17"/>
+        <v>14</v>
+      </c>
+      <c r="H48" t="s">
+        <v>22</v>
       </c>
       <c r="I48">
-        <f>(2/3)*$B48*((13-E48)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="18"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J48">
-        <f>(2/3)*$B48*((13-F48)/12)</f>
+        <f t="shared" si="19"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K48">
-        <f>I48+J48</f>
-        <v>0.61111111111111116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49">
-        <v>2</v>
-      </c>
-      <c r="C49">
-        <v>24</v>
-      </c>
-      <c r="D49">
-        <f>(24-C49)/12</f>
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>5</v>
-      </c>
-      <c r="F49">
-        <v>8</v>
-      </c>
-      <c r="G49">
-        <f>SUM(D49:F49)/B49</f>
-        <v>6.5</v>
-      </c>
-      <c r="I49">
-        <f>(2/3)*$B49*((13-E49)/12)</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="J49">
-        <f>(2/3)*$B49*((13-F49)/12)</f>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="K49">
-        <f>I49+J49</f>
-        <v>1.4444444444444444</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
       <c r="C50">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D50">
-        <f>(24-C50)/12</f>
-        <v>-1</v>
+        <f t="shared" ref="D50:K60" si="22">(24-C50)/12</f>
+        <v>-2</v>
       </c>
       <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>7</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ref="G50:G56" si="23">SUM(D50:F50)/B50</f>
+        <v>6.5</v>
+      </c>
+      <c r="I50">
+        <f t="shared" ref="I50:J58" si="24">(2/3)*$B50*((13-E50)/12)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="24"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K50">
+        <f t="shared" ref="K50:K58" si="25">I50+J50</f>
+        <v>1.2222222222222223</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>48</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="22"/>
+        <v>-2</v>
+      </c>
+      <c r="E51">
+        <v>7</v>
+      </c>
+      <c r="F51">
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="23"/>
+        <v>13</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="24"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="24"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="25"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>24</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="E52">
         <v>5</v>
-      </c>
-      <c r="F50">
-        <v>9</v>
-      </c>
-      <c r="G50">
-        <f>SUM(D50:F50)/B50</f>
-        <v>6.5</v>
-      </c>
-      <c r="I50">
-        <f>(2/3)*$B50*((13-E50)/12)</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="J50">
-        <f>(2/3)*$B50*((13-F50)/12)</f>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="K50">
-        <f>I50+J50</f>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>24</v>
-      </c>
-      <c r="D51">
-        <f>(24-C51)/12</f>
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>9</v>
-      </c>
-      <c r="F51">
-        <v>4</v>
-      </c>
-      <c r="G51">
-        <f>SUM(D51:F51)/B51</f>
-        <v>13</v>
-      </c>
-      <c r="I51">
-        <f>(2/3)*$B51*((13-E51)/12)</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="J51">
-        <f>(2/3)*$B51*((13-F51)/12)</f>
-        <v>0.5</v>
-      </c>
-      <c r="K51">
-        <f>I51+J51</f>
-        <v>0.72222222222222221</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>36</v>
-      </c>
-      <c r="D52">
-        <f>(24-C52)/12</f>
-        <v>-1</v>
-      </c>
-      <c r="E52">
-        <v>6</v>
       </c>
       <c r="F52">
         <v>8</v>
       </c>
       <c r="G52">
-        <f>SUM(D52:F52)/B52</f>
-        <v>13</v>
+        <f t="shared" si="23"/>
+        <v>6.5</v>
       </c>
       <c r="I52">
-        <f>(2/3)*$B52*((13-E52)/12)</f>
-        <v>0.3888888888888889</v>
+        <f t="shared" si="24"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J52">
-        <f>(2/3)*$B52*((13-F52)/12)</f>
-        <v>0.27777777777777779</v>
+        <f t="shared" si="24"/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="K52">
-        <f>I52+J52</f>
-        <v>0.66666666666666674</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>1.4444444444444444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
       <c r="C53">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D53">
-        <f>(24-C53)/12</f>
-        <v>-2</v>
+        <f t="shared" si="22"/>
+        <v>-1</v>
       </c>
       <c r="E53">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F53">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G53">
-        <f>SUM(D53:F53)/B53</f>
+        <f t="shared" si="23"/>
         <v>6.5</v>
       </c>
       <c r="I53">
-        <f>(2/3)*$B53*((13-E53)/12)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="24"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J53">
-        <f>(2/3)*$B53*((13-F53)/12)</f>
-        <v>0.88888888888888884</v>
+        <f t="shared" si="24"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="K53">
-        <f>I53+J53</f>
-        <v>1.2222222222222221</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D54">
-        <f>(24-C54)/12</f>
-        <v>1</v>
+        <f t="shared" si="22"/>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="23"/>
+        <v>13</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="24"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="24"/>
+        <v>0.5</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="25"/>
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>36</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="22"/>
+        <v>-1</v>
+      </c>
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
         <v>8</v>
       </c>
-      <c r="G54">
-        <f t="shared" ref="G54:G57" si="9">SUM(D54:F54)/B54</f>
-        <v>7</v>
-      </c>
-      <c r="H54" t="s">
-        <v>22</v>
-      </c>
-      <c r="I54">
-        <f>(2/3)*$B54*((13-E54)/12)</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="J54">
-        <f>(2/3)*$B54*((13-F54)/12)</f>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="K54">
-        <f>I54+J54</f>
-        <v>1.4444444444444444</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <f t="shared" si="23"/>
+        <v>13</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="24"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="24"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="25"/>
+        <v>0.66666666666666674</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -2421,78 +2488,306 @@
         <v>48</v>
       </c>
       <c r="D56">
-        <f t="shared" ref="D55:D57" si="10">(24-C56)/12</f>
+        <f t="shared" si="22"/>
         <v>-2</v>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F56">
+        <v>5</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="23"/>
+        <v>6.5</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="24"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="24"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="25"/>
+        <v>1.2222222222222221</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>8</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ref="G57:G60" si="26">SUM(D57:F57)/B57</f>
+        <v>7</v>
+      </c>
+      <c r="H57" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="24"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="24"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="25"/>
+        <v>1.4444444444444444</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>48</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="22"/>
+        <v>-2</v>
+      </c>
+      <c r="E58">
+        <v>10</v>
+      </c>
+      <c r="F58">
+        <v>5</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="26"/>
+        <v>6.5</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="24"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="24"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="25"/>
+        <v>1.2222222222222221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>18</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="E59">
+        <v>6</v>
+      </c>
+      <c r="F59">
         <v>11</v>
       </c>
-      <c r="G56">
-        <f t="shared" si="9"/>
+      <c r="G59">
+        <f t="shared" si="26"/>
+        <v>4.375</v>
+      </c>
+      <c r="I59">
+        <f t="shared" ref="I59:I60" si="27">(2/3)*$B59*((13-E59)/12)</f>
+        <v>1.5555555555555556</v>
+      </c>
+      <c r="J59">
+        <f t="shared" ref="J59:J60" si="28">(2/3)*$B59*((13-F59)/12)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="K59">
+        <f t="shared" ref="K59:K60" si="29">I59+J59</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>18</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="E60">
+        <v>6</v>
+      </c>
+      <c r="F60">
         <v>8</v>
       </c>
-      <c r="H56" t="s">
-        <v>57</v>
-      </c>
-      <c r="I56">
-        <f t="shared" ref="I55:I57" si="11">(2/3)*$B56*((13-E56)/12)</f>
+      <c r="G60">
+        <f t="shared" si="26"/>
+        <v>7.25</v>
+      </c>
+      <c r="I60">
+        <f t="shared" ref="I60:I63" si="30">(2/3)*$B60*((13-E60)/12)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="J60">
+        <f t="shared" ref="J60:J63" si="31">(2/3)*$B60*((13-F60)/12)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K60">
+        <f t="shared" ref="K60:K63" si="32">I60+J60</f>
+        <v>1.3333333333333335</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>36</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ref="D61:K63" si="33">(24-C61)/12</f>
+        <v>-1</v>
+      </c>
+      <c r="E61">
+        <v>6</v>
+      </c>
+      <c r="F61">
+        <v>7</v>
+      </c>
+      <c r="G61">
+        <f>SUM(D61:F61)/B61</f>
+        <v>6</v>
+      </c>
+      <c r="H61" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="30"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="31"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J56">
-        <f t="shared" ref="J55:J57" si="12">(2/3)*$B56*((13-F56)/12)</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="K56">
-        <f t="shared" ref="K55:K57" si="13">I56+J56</f>
+      <c r="K61">
+        <f t="shared" si="32"/>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="M61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>36</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="33"/>
+        <v>-1</v>
+      </c>
+      <c r="E62">
+        <v>7</v>
+      </c>
+      <c r="F62">
+        <v>7</v>
+      </c>
+      <c r="G62">
+        <f>SUM(D62:F62)/B62</f>
+        <v>6.5</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="30"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="31"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="32"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>24</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>7</v>
+      </c>
+      <c r="F63">
+        <v>5</v>
+      </c>
+      <c r="G63">
+        <f>SUM(D63:F63)/B63</f>
+        <v>6</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="30"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="31"/>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>72</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="10"/>
-        <v>-4</v>
-      </c>
-      <c r="E57">
-        <v>7</v>
-      </c>
-      <c r="F57">
-        <v>6</v>
-      </c>
-      <c r="G57">
-        <f t="shared" si="9"/>
-        <v>9</v>
-      </c>
-      <c r="H57" t="s">
-        <v>57</v>
-      </c>
-      <c r="I57">
-        <f t="shared" si="11"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="J57">
-        <f t="shared" si="12"/>
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="K57">
-        <f t="shared" si="13"/>
-        <v>0.72222222222222221</v>
+      <c r="K63">
+        <f t="shared" si="32"/>
+        <v>1.5555555555555554</v>
+      </c>
+      <c r="L63">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G32">
-    <sortCondition ref="C1:C32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G35">
+    <sortCondition ref="C1:C35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Buffed HQ choices and walkers, edited nids
</commit_message>
<xml_diff>
--- a/Raw Data/weapons.xlsx
+++ b/Raw Data/weapons.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahoan\Documents\github\40kLite\40klite\Raw Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Battlescribe\github\40klite\40klite\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F990A1-F401-4280-B715-7FD9821BE3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B422A801-EAA8-4E32-B4F1-D135728C0503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -756,13 +756,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
+      <selection pane="bottomLeft" activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1630,7 +1631,7 @@
         <v>5</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:I23" si="16">(2/3)*$B22*((13-E22)/12)</f>
+        <f t="shared" ref="I22" si="16">(2/3)*$B22*((13-E22)/12)</f>
         <v>0.5</v>
       </c>
       <c r="J22">
@@ -1939,6 +1940,15 @@
       <c r="K29">
         <f t="shared" si="24"/>
         <v>1.4444444444444444</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed points and updated profiles
</commit_message>
<xml_diff>
--- a/Raw Data/weapons.xlsx
+++ b/Raw Data/weapons.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Battlescribe\github\40klite\40klite\Raw Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahoan\Documents\github\40kLite\40klite\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B422A801-EAA8-4E32-B4F1-D135728C0503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F356EE9-D738-4A13-95DB-2FD4052721B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
   <si>
     <t>Weapon</t>
   </si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t>Stranglethorn</t>
+  </si>
+  <si>
+    <t>Assault Bolter</t>
+  </si>
+  <si>
+    <t>Heavy Onslaught</t>
+  </si>
+  <si>
+    <t>Laser Destroyer</t>
   </si>
 </sst>
 </file>
@@ -752,11 +761,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFAFC17-B8CC-4FDE-905B-FC2D8F8BC7C4}">
-  <dimension ref="A1:U76"/>
+  <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N29" sqref="N29"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,6 +3504,151 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <v>18</v>
+      </c>
+      <c r="E78">
+        <v>4</v>
+      </c>
+      <c r="F78">
+        <v>10</v>
+      </c>
+      <c r="I78">
+        <f t="shared" ref="I77:I79" si="57">(2/3)*$B78*((13-E78)/12)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J78">
+        <f t="shared" ref="J77:J79" si="58">(2/3)*$B78*((13-F78)/12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K78">
+        <f t="shared" ref="K77:K79" si="59">I78+J78</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79">
+        <v>18</v>
+      </c>
+      <c r="E79">
+        <v>7</v>
+      </c>
+      <c r="F79">
+        <v>7</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="57"/>
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="58"/>
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="59"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>95</v>
+      </c>
+      <c r="B81">
+        <v>3</v>
+      </c>
+      <c r="C81">
+        <v>30</v>
+      </c>
+      <c r="E81">
+        <v>6</v>
+      </c>
+      <c r="F81">
+        <v>9</v>
+      </c>
+      <c r="I81">
+        <f t="shared" ref="I80:I83" si="60">(2/3)*$B81*((13-E81)/12)</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J81">
+        <f t="shared" ref="J80:J83" si="61">(2/3)*$B81*((13-F81)/12)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K81">
+        <f t="shared" ref="K80:K83" si="62">I81+J81</f>
+        <v>1.8333333333333335</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82">
+        <v>36</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+      <c r="F82">
+        <v>5</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="60"/>
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="61"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="62"/>
+        <v>1.8888888888888888</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>96</v>
+      </c>
+      <c r="B83">
+        <v>3</v>
+      </c>
+      <c r="C83">
+        <v>72</v>
+      </c>
+      <c r="E83">
+        <v>11</v>
+      </c>
+      <c r="F83">
+        <v>5</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="60"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="61"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="62"/>
+        <v>1.6666666666666665</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G40">
     <sortCondition ref="C1:C40"/>

</xml_diff>

<commit_message>
Updated Guard Super Heavies
</commit_message>
<xml_diff>
--- a/Raw Data/weapons.xlsx
+++ b/Raw Data/weapons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Battlescribe\github\40klite\40klite\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAEA4B2-5FE1-459A-AE00-1FB5820FFDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B8CC6A-C678-4696-9656-137A391E97EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
   <si>
     <t>Weapon</t>
   </si>
@@ -342,6 +342,30 @@
   </si>
   <si>
     <t>Shoota</t>
+  </si>
+  <si>
+    <t>Baneblade Cannon</t>
+  </si>
+  <si>
+    <t>Hellhammer</t>
+  </si>
+  <si>
+    <t>Tremor Cannon</t>
+  </si>
+  <si>
+    <t>Quake Cannon</t>
+  </si>
+  <si>
+    <t>Magma</t>
+  </si>
+  <si>
+    <t>Volcano</t>
+  </si>
+  <si>
+    <t>Stormsword</t>
+  </si>
+  <si>
+    <t>Vulcan</t>
   </si>
 </sst>
 </file>
@@ -385,9 +409,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,11 +801,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFAFC17-B8CC-4FDE-905B-FC2D8F8BC7C4}">
-  <dimension ref="A1:U91"/>
+  <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,7 +2111,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -2123,7 +2148,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2160,7 +2185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2197,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -2234,7 +2259,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2271,7 +2296,7 @@
         <v>0.61111111111111105</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2308,7 +2333,7 @@
         <v>0.72222222222222221</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2345,7 +2370,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2381,8 +2406,9 @@
         <f t="shared" si="31"/>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T41" s="2"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2419,7 +2445,7 @@
         <v>0.61111111111111116</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2456,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G44" t="e">
         <f t="shared" si="28"/>
         <v>#DIV/0!</v>
@@ -2474,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -2519,7 +2545,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -2556,7 +2582,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -2593,7 +2619,7 @@
         <v>0.72222222222222221</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -3785,15 +3811,15 @@
         <v>7</v>
       </c>
       <c r="I90">
-        <f t="shared" ref="I89:I90" si="66">(2/3)*$B90*((13-E90)/12)</f>
+        <f t="shared" ref="I90" si="66">(2/3)*$B90*((13-E90)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J90">
-        <f t="shared" ref="J89:J90" si="67">(2/3)*$B90*((13-F90)/12)</f>
+        <f t="shared" ref="J90" si="67">(2/3)*$B90*((13-F90)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="K90">
-        <f t="shared" ref="K89:K90" si="68">I90+J90</f>
+        <f t="shared" ref="K90" si="68">I90+J90</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -3824,6 +3850,238 @@
       <c r="K91">
         <f t="shared" ref="K91" si="71">I91+J91</f>
         <v>0.77777777777777768</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <v>72</v>
+      </c>
+      <c r="E93">
+        <v>5</v>
+      </c>
+      <c r="F93">
+        <v>6</v>
+      </c>
+      <c r="I93">
+        <f t="shared" ref="I92:I94" si="72">(2/3)*$B93*((13-E93)/12)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J93">
+        <f t="shared" ref="J92:J94" si="73">(2/3)*$B93*((13-F93)/12)</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="K93">
+        <f t="shared" ref="K92:K94" si="74">I93+J93</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>103</v>
+      </c>
+      <c r="B94">
+        <v>3</v>
+      </c>
+      <c r="C94">
+        <v>36</v>
+      </c>
+      <c r="E94">
+        <v>4</v>
+      </c>
+      <c r="F94">
+        <v>5</v>
+      </c>
+      <c r="I94">
+        <f t="shared" ref="I94:I99" si="75">(2/3)*$B94*((13-E94)/12)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J94">
+        <f t="shared" ref="J94:J99" si="76">(2/3)*$B94*((13-F94)/12)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="K94">
+        <f t="shared" ref="K94:K99" si="77">I94+J94</f>
+        <v>2.833333333333333</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95">
+        <v>3</v>
+      </c>
+      <c r="C95">
+        <v>60</v>
+      </c>
+      <c r="E95">
+        <v>6</v>
+      </c>
+      <c r="F95">
+        <v>7</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="75"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="77"/>
+        <v>2.166666666666667</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96">
+        <v>140</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
+      </c>
+      <c r="F96">
+        <v>3</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="75"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="76"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="77"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>106</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97">
+        <v>60</v>
+      </c>
+      <c r="E97">
+        <v>5</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="75"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="76"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="77"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+      <c r="C98">
+        <v>120</v>
+      </c>
+      <c r="E98">
+        <v>8</v>
+      </c>
+      <c r="F98">
+        <v>3</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="75"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="76"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K98">
+        <f t="shared" si="77"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99">
+        <v>3</v>
+      </c>
+      <c r="C99">
+        <v>36</v>
+      </c>
+      <c r="E99">
+        <v>4</v>
+      </c>
+      <c r="F99">
+        <v>6</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="75"/>
+        <v>1.5</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="76"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="K99">
+        <f t="shared" si="77"/>
+        <v>2.666666666666667</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>109</v>
+      </c>
+      <c r="B100">
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <v>60</v>
+      </c>
+      <c r="E100">
+        <v>6</v>
+      </c>
+      <c r="F100">
+        <v>8</v>
+      </c>
+      <c r="I100">
+        <f t="shared" ref="I100" si="78">(2/3)*$B100*((13-E100)/12)</f>
+        <v>1.5555555555555556</v>
+      </c>
+      <c r="J100">
+        <f t="shared" ref="J100" si="79">(2/3)*$B100*((13-F100)/12)</f>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="K100">
+        <f t="shared" ref="K100" si="80">I100+J100</f>
+        <v>2.666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Tervigons and added Knights + Necrons
</commit_message>
<xml_diff>
--- a/Raw Data/weapons.xlsx
+++ b/Raw Data/weapons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Battlescribe\github\40klite\40klite\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B8CC6A-C678-4696-9656-137A391E97EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F1951C-FE25-4C38-AFB8-AEE715188026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
   <si>
     <t>Weapon</t>
   </si>
@@ -366,6 +366,39 @@
   </si>
   <si>
     <t>Vulcan</t>
+  </si>
+  <si>
+    <t>Las-Impulsor</t>
+  </si>
+  <si>
+    <t>Plasma Destructor</t>
+  </si>
+  <si>
+    <t>Shieldbreaker Cannon</t>
+  </si>
+  <si>
+    <t>Missile</t>
+  </si>
+  <si>
+    <t>Gauntlet</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Ironstorm</t>
+  </si>
+  <si>
+    <t>Stormspear</t>
+  </si>
+  <si>
+    <t>Twin Icarus</t>
+  </si>
+  <si>
+    <t>Tesla cannon</t>
+  </si>
+  <si>
+    <t>Gauss Cannon</t>
   </si>
 </sst>
 </file>
@@ -801,11 +834,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFAFC17-B8CC-4FDE-905B-FC2D8F8BC7C4}">
-  <dimension ref="A1:U100"/>
+  <dimension ref="A1:V115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,7 +2892,7 @@
         <v>48</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55:D65" si="33">(24-C55)/12</f>
+        <f t="shared" ref="D55:D67" si="33">(24-C55)/12</f>
         <v>-2</v>
       </c>
       <c r="E55">
@@ -3132,7 +3165,7 @@
         <v>8</v>
       </c>
       <c r="G62">
-        <f t="shared" ref="G62:G65" si="37">SUM(D62:F62)/B62</f>
+        <f t="shared" ref="G62:G66" si="37">SUM(D62:F62)/B62</f>
         <v>7</v>
       </c>
       <c r="H62" t="s">
@@ -3225,7 +3258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -3250,41 +3283,53 @@
         <v>7.25</v>
       </c>
       <c r="I65">
-        <f t="shared" ref="I65:I68" si="41">(2/3)*$B65*((13-E65)/12)</f>
+        <f t="shared" ref="I65:I70" si="41">(2/3)*$B65*((13-E65)/12)</f>
         <v>0.77777777777777779</v>
       </c>
       <c r="J65">
-        <f t="shared" ref="J65:J68" si="42">(2/3)*$B65*((13-F65)/12)</f>
+        <f t="shared" ref="J65:J70" si="42">(2/3)*$B65*((13-F65)/12)</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="K65">
-        <f t="shared" ref="K65:K68" si="43">I65+J65</f>
+        <f t="shared" ref="K65:K70" si="43">I65+J65</f>
         <v>1.3333333333333335</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S65">
+        <v>7</v>
+      </c>
+      <c r="T65">
+        <v>14</v>
+      </c>
+      <c r="U65">
+        <v>21</v>
+      </c>
+      <c r="V65">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>119</v>
+      </c>
       <c r="B66">
         <v>2</v>
       </c>
       <c r="C66">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D68" si="44">(24-C66)/12</f>
-        <v>-1</v>
+        <f t="shared" si="33"/>
+        <v>-0.5</v>
       </c>
       <c r="E66">
         <v>6</v>
       </c>
       <c r="F66">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G66">
-        <f>SUM(D66:F66)/B66</f>
-        <v>6</v>
-      </c>
-      <c r="H66" t="s">
-        <v>22</v>
+        <f t="shared" si="37"/>
+        <v>6.75</v>
       </c>
       <c r="I66">
         <f t="shared" si="41"/>
@@ -3292,157 +3337,169 @@
       </c>
       <c r="J66">
         <f t="shared" si="42"/>
-        <v>0.66666666666666663</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="K66">
         <f t="shared" si="43"/>
+        <v>1.3333333333333335</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>24</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>7</v>
+      </c>
+      <c r="F67">
+        <v>6</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67" si="44">(2/3)*$B67*((13-E67)/12)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J67">
+        <f t="shared" ref="J67" si="45">(2/3)*$B67*((13-F67)/12)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="K67">
+        <f t="shared" ref="K67" si="46">I67+J67</f>
         <v>1.4444444444444444</v>
       </c>
-      <c r="M66" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67">
-        <v>2</v>
-      </c>
-      <c r="C67">
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
         <v>36</v>
       </c>
-      <c r="D67">
-        <f t="shared" si="44"/>
+      <c r="D68">
+        <f t="shared" ref="D68:D70" si="47">(24-C68)/12</f>
         <v>-1</v>
       </c>
-      <c r="E67">
-        <v>7</v>
-      </c>
-      <c r="F67">
-        <v>7</v>
-      </c>
-      <c r="G67">
-        <f>SUM(D67:F67)/B67</f>
-        <v>6.5</v>
-      </c>
-      <c r="I67">
-        <f t="shared" si="41"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J67">
-        <f t="shared" si="42"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="K67">
-        <f t="shared" si="43"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="L67" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68">
-        <v>2</v>
-      </c>
-      <c r="C68">
-        <v>24</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
       <c r="E68">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G68">
         <f>SUM(D68:F68)/B68</f>
         <v>6</v>
       </c>
+      <c r="H68" t="s">
+        <v>22</v>
+      </c>
       <c r="I68">
         <f t="shared" si="41"/>
-        <v>0.66666666666666663</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="J68">
         <f t="shared" si="42"/>
-        <v>0.88888888888888884</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K68">
         <f t="shared" si="43"/>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="M68" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69">
+        <v>36</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="47"/>
+        <v>-1</v>
+      </c>
+      <c r="E69">
+        <v>7</v>
+      </c>
+      <c r="F69">
+        <v>7</v>
+      </c>
+      <c r="G69">
+        <f>SUM(D69:F69)/B69</f>
+        <v>6.5</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="41"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="42"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="43"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70">
+        <v>24</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>7</v>
+      </c>
+      <c r="F70">
+        <v>5</v>
+      </c>
+      <c r="G70">
+        <f>SUM(D70:F70)/B70</f>
+        <v>6</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="41"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="42"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="43"/>
         <v>1.5555555555555554</v>
       </c>
-      <c r="L68">
+      <c r="L70">
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>85</v>
-      </c>
-      <c r="B70">
-        <v>2</v>
-      </c>
-      <c r="C70">
-        <v>48</v>
-      </c>
-      <c r="E70">
-        <v>7</v>
-      </c>
-      <c r="F70">
-        <v>8</v>
-      </c>
-      <c r="I70">
-        <f t="shared" ref="I70" si="45">(2/3)*$B70*((13-E70)/12)</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J70">
-        <f t="shared" ref="J70" si="46">(2/3)*$B70*((13-F70)/12)</f>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="K70">
-        <f t="shared" ref="K70" si="47">I70+J70</f>
-        <v>1.2222222222222223</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>86</v>
-      </c>
-      <c r="B71">
-        <v>4</v>
-      </c>
-      <c r="C71">
-        <v>24</v>
-      </c>
-      <c r="E71">
-        <v>7</v>
-      </c>
-      <c r="F71">
-        <v>12</v>
-      </c>
-      <c r="I71">
-        <f t="shared" ref="I71:I72" si="48">(2/3)*$B71*((13-E71)/12)</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="J71">
-        <f t="shared" ref="J71:J72" si="49">(2/3)*$B71*((13-F71)/12)</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="K71">
-        <f t="shared" ref="K71:K72" si="50">I71+J71</f>
-        <v>1.5555555555555554</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>87</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -3451,637 +3508,987 @@
         <v>48</v>
       </c>
       <c r="E72">
+        <v>7</v>
+      </c>
+      <c r="F72">
+        <v>8</v>
+      </c>
+      <c r="I72">
+        <f t="shared" ref="I72" si="48">(2/3)*$B72*((13-E72)/12)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J72">
+        <f t="shared" ref="J72" si="49">(2/3)*$B72*((13-F72)/12)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K72">
+        <f t="shared" ref="K72" si="50">I72+J72</f>
+        <v>1.2222222222222223</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <v>24</v>
+      </c>
+      <c r="E73">
+        <v>7</v>
+      </c>
+      <c r="F73">
+        <v>12</v>
+      </c>
+      <c r="I73">
+        <f t="shared" ref="I73:I74" si="51">(2/3)*$B73*((13-E73)/12)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J73">
+        <f t="shared" ref="J73:J74" si="52">(2/3)*$B73*((13-F73)/12)</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K73">
+        <f t="shared" ref="K73:K74" si="53">I73+J73</f>
+        <v>1.5555555555555554</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>48</v>
+      </c>
+      <c r="E74">
         <v>9</v>
       </c>
-      <c r="F72">
+      <c r="F74">
         <v>6</v>
       </c>
-      <c r="I72">
-        <f t="shared" si="48"/>
+      <c r="I74">
+        <f t="shared" si="51"/>
         <v>0.44444444444444442</v>
       </c>
-      <c r="J72">
-        <f t="shared" si="49"/>
+      <c r="J74">
+        <f t="shared" si="52"/>
         <v>0.77777777777777779</v>
       </c>
-      <c r="K72">
-        <f t="shared" si="50"/>
+      <c r="K74">
+        <f t="shared" si="53"/>
         <v>1.2222222222222223</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>88</v>
       </c>
-      <c r="B74">
+      <c r="B76">
         <v>3</v>
       </c>
-      <c r="E74">
+      <c r="E76">
         <v>5</v>
       </c>
-      <c r="F74">
+      <c r="F76">
         <v>9</v>
       </c>
-      <c r="L74">
+      <c r="L76">
         <f>3*(2/3)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>89</v>
       </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-      <c r="C75">
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
         <v>24</v>
       </c>
-      <c r="E75">
+      <c r="E77">
         <v>8</v>
       </c>
-      <c r="F75">
+      <c r="F77">
         <v>10</v>
       </c>
-      <c r="I75">
-        <f t="shared" ref="I75" si="51">(2/3)*$B75*((13-E75)/12)</f>
+      <c r="I77">
+        <f t="shared" ref="I77" si="54">(2/3)*$B77*((13-E77)/12)</f>
         <v>0.27777777777777779</v>
       </c>
-      <c r="J75">
-        <f t="shared" ref="J75" si="52">(2/3)*$B75*((13-F75)/12)</f>
+      <c r="J77">
+        <f t="shared" ref="J77" si="55">(2/3)*$B77*((13-F77)/12)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="K75">
-        <f t="shared" ref="K75" si="53">I75+J75</f>
+      <c r="K77">
+        <f t="shared" ref="K77" si="56">I77+J77</f>
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>90</v>
       </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76">
-        <v>18</v>
-      </c>
-      <c r="E76">
-        <v>6</v>
-      </c>
-      <c r="F76">
-        <v>11</v>
-      </c>
-      <c r="I76">
-        <f t="shared" ref="I76" si="54">(2/3)*$B76*((13-E76)/12)</f>
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="J76">
-        <f t="shared" ref="J76" si="55">(2/3)*$B76*((13-F76)/12)</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="K76">
-        <f t="shared" ref="K76" si="56">I76+J76</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>94</v>
-      </c>
       <c r="B78">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>18</v>
       </c>
       <c r="E78">
+        <v>6</v>
+      </c>
+      <c r="F78">
+        <v>11</v>
+      </c>
+      <c r="I78">
+        <f t="shared" ref="I78" si="57">(2/3)*$B78*((13-E78)/12)</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="J78">
+        <f t="shared" ref="J78" si="58">(2/3)*$B78*((13-F78)/12)</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K78">
+        <f t="shared" ref="K78" si="59">I78+J78</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80">
+        <v>3</v>
+      </c>
+      <c r="C80">
+        <v>18</v>
+      </c>
+      <c r="E80">
         <v>4</v>
       </c>
-      <c r="F78">
+      <c r="F80">
         <v>10</v>
       </c>
-      <c r="I78">
-        <f t="shared" ref="I78:I79" si="57">(2/3)*$B78*((13-E78)/12)</f>
+      <c r="I80">
+        <f t="shared" ref="I80:I81" si="60">(2/3)*$B80*((13-E80)/12)</f>
         <v>1.5</v>
       </c>
-      <c r="J78">
-        <f t="shared" ref="J78:J79" si="58">(2/3)*$B78*((13-F78)/12)</f>
+      <c r="J80">
+        <f t="shared" ref="J80:J81" si="61">(2/3)*$B80*((13-F80)/12)</f>
         <v>0.5</v>
       </c>
-      <c r="K78">
-        <f t="shared" ref="K78:K79" si="59">I78+J78</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79">
-        <v>3</v>
-      </c>
-      <c r="C79">
-        <v>18</v>
-      </c>
-      <c r="E79">
-        <v>7</v>
-      </c>
-      <c r="F79">
-        <v>7</v>
-      </c>
-      <c r="I79">
-        <f t="shared" si="57"/>
-        <v>1</v>
-      </c>
-      <c r="J79">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="K79">
-        <f t="shared" si="59"/>
+      <c r="K80">
+        <f t="shared" ref="K80:K81" si="62">I80+J80</f>
         <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="B81">
         <v>3</v>
       </c>
       <c r="C81">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E81">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I81">
-        <f t="shared" ref="I81:I83" si="60">(2/3)*$B81*((13-E81)/12)</f>
-        <v>1.1666666666666667</v>
+        <f t="shared" si="60"/>
+        <v>1</v>
       </c>
       <c r="J81">
-        <f t="shared" ref="J81:J83" si="61">(2/3)*$B81*((13-F81)/12)</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="61"/>
+        <v>1</v>
       </c>
       <c r="K81">
-        <f t="shared" ref="K81:K83" si="62">I81+J81</f>
-        <v>1.8333333333333335</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>9</v>
-      </c>
-      <c r="B82">
-        <v>2</v>
-      </c>
-      <c r="C82">
-        <v>36</v>
-      </c>
-      <c r="E82">
-        <v>4</v>
-      </c>
-      <c r="F82">
-        <v>5</v>
-      </c>
-      <c r="I82">
-        <f t="shared" si="60"/>
-        <v>1</v>
-      </c>
-      <c r="J82">
-        <f t="shared" si="61"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="K82">
         <f t="shared" si="62"/>
-        <v>1.8888888888888888</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B83">
         <v>3</v>
       </c>
       <c r="C83">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="E83">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F83">
+        <v>9</v>
+      </c>
+      <c r="I83">
+        <f t="shared" ref="I83:I85" si="63">(2/3)*$B83*((13-E83)/12)</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J83">
+        <f t="shared" ref="J83:J85" si="64">(2/3)*$B83*((13-F83)/12)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K83">
+        <f t="shared" ref="K83:K85" si="65">I83+J83</f>
+        <v>1.8333333333333335</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84">
+        <v>36</v>
+      </c>
+      <c r="E84">
+        <v>4</v>
+      </c>
+      <c r="F84">
         <v>5</v>
       </c>
-      <c r="I83">
-        <f t="shared" si="60"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="J83">
-        <f t="shared" si="61"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="K83">
-        <f t="shared" si="62"/>
-        <v>1.6666666666666665</v>
+      <c r="I84">
+        <f t="shared" si="63"/>
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="64"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="65"/>
+        <v>1.8888888888888888</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B85">
         <v>3</v>
       </c>
+      <c r="C85">
+        <v>72</v>
+      </c>
       <c r="E85">
+        <v>11</v>
+      </c>
+      <c r="F85">
         <v>5</v>
       </c>
-      <c r="F85">
-        <v>7</v>
-      </c>
       <c r="I85">
-        <f t="shared" ref="I85:I88" si="63">(2/3)*$B85*((13-E85)/12)</f>
+        <f t="shared" si="63"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="64"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="J85">
-        <f t="shared" ref="J85:J88" si="64">(2/3)*$B85*((13-F85)/12)</f>
-        <v>1</v>
-      </c>
       <c r="K85">
-        <f t="shared" ref="K85:K88" si="65">I85+J85</f>
-        <v>2.333333333333333</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86">
-        <v>2</v>
-      </c>
-      <c r="E86">
-        <v>8</v>
-      </c>
-      <c r="F86">
-        <v>4</v>
-      </c>
-      <c r="I86">
-        <f t="shared" si="63"/>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="J86">
-        <f t="shared" si="64"/>
-        <v>1</v>
-      </c>
-      <c r="K86">
         <f t="shared" si="65"/>
-        <v>1.5555555555555556</v>
+        <v>1.6666666666666665</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E87">
         <v>5</v>
       </c>
       <c r="F87">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I87">
-        <f t="shared" si="63"/>
-        <v>1.7777777777777777</v>
+        <f t="shared" ref="I87:I90" si="66">(2/3)*$B87*((13-E87)/12)</f>
+        <v>1.3333333333333333</v>
       </c>
       <c r="J87">
-        <f t="shared" si="64"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" ref="J87:J90" si="67">(2/3)*$B87*((13-F87)/12)</f>
+        <v>1</v>
       </c>
       <c r="K87">
-        <f t="shared" si="65"/>
-        <v>2.4444444444444442</v>
+        <f t="shared" ref="K87:K90" si="68">I87+J87</f>
+        <v>2.333333333333333</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E88">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F88">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I88">
-        <f t="shared" si="63"/>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="66"/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="J88">
-        <f t="shared" si="64"/>
-        <v>0.27777777777777779</v>
+        <f t="shared" si="67"/>
+        <v>1</v>
       </c>
       <c r="K88">
-        <f t="shared" si="65"/>
-        <v>0.61111111111111116</v>
+        <f t="shared" si="68"/>
+        <v>1.5555555555555556</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>99</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="E89">
+        <v>5</v>
+      </c>
+      <c r="F89">
+        <v>10</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="66"/>
+        <v>1.7777777777777777</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="67"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="68"/>
+        <v>2.4444444444444442</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>7</v>
+      </c>
+      <c r="F90">
+        <v>8</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="66"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="67"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="68"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>100</v>
       </c>
-      <c r="B90">
-        <v>2</v>
-      </c>
-      <c r="C90">
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92">
         <v>24</v>
       </c>
-      <c r="E90">
-        <v>7</v>
-      </c>
-      <c r="F90">
-        <v>7</v>
-      </c>
-      <c r="I90">
-        <f t="shared" ref="I90" si="66">(2/3)*$B90*((13-E90)/12)</f>
+      <c r="E92">
+        <v>7</v>
+      </c>
+      <c r="F92">
+        <v>7</v>
+      </c>
+      <c r="I92">
+        <f t="shared" ref="I92" si="69">(2/3)*$B92*((13-E92)/12)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J90">
-        <f t="shared" ref="J90" si="67">(2/3)*$B90*((13-F90)/12)</f>
+      <c r="J92">
+        <f t="shared" ref="J92" si="70">(2/3)*$B92*((13-F92)/12)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="K90">
-        <f t="shared" ref="K90" si="68">I90+J90</f>
+      <c r="K92">
+        <f t="shared" ref="K92" si="71">I92+J92</f>
         <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>101</v>
-      </c>
-      <c r="B91">
-        <v>2</v>
-      </c>
-      <c r="C91">
-        <v>36</v>
-      </c>
-      <c r="E91">
-        <v>7</v>
-      </c>
-      <c r="F91">
-        <v>12</v>
-      </c>
-      <c r="I91">
-        <f t="shared" ref="I91" si="69">(2/3)*$B91*((13-E91)/12)</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J91">
-        <f t="shared" ref="J91" si="70">(2/3)*$B91*((13-F91)/12)</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="K91">
-        <f t="shared" ref="K91" si="71">I91+J91</f>
-        <v>0.77777777777777768</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="E93">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F93">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I93">
-        <f t="shared" ref="I92:I94" si="72">(2/3)*$B93*((13-E93)/12)</f>
-        <v>1.3333333333333333</v>
+        <f t="shared" ref="I93" si="72">(2/3)*$B93*((13-E93)/12)</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J93">
-        <f t="shared" ref="J92:J94" si="73">(2/3)*$B93*((13-F93)/12)</f>
-        <v>1.1666666666666667</v>
+        <f t="shared" ref="J93" si="73">(2/3)*$B93*((13-F93)/12)</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K93">
-        <f t="shared" ref="K92:K94" si="74">I93+J93</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>103</v>
-      </c>
-      <c r="B94">
-        <v>3</v>
-      </c>
-      <c r="C94">
-        <v>36</v>
-      </c>
-      <c r="E94">
-        <v>4</v>
-      </c>
-      <c r="F94">
-        <v>5</v>
-      </c>
-      <c r="I94">
-        <f t="shared" ref="I94:I99" si="75">(2/3)*$B94*((13-E94)/12)</f>
-        <v>1.5</v>
-      </c>
-      <c r="J94">
-        <f t="shared" ref="J94:J99" si="76">(2/3)*$B94*((13-F94)/12)</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="K94">
-        <f t="shared" ref="K94:K99" si="77">I94+J94</f>
-        <v>2.833333333333333</v>
+        <f t="shared" ref="K93" si="74">I93+J93</f>
+        <v>0.77777777777777768</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B95">
         <v>3</v>
       </c>
       <c r="C95">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E95">
+        <v>5</v>
+      </c>
+      <c r="F95">
         <v>6</v>
       </c>
-      <c r="F95">
-        <v>7</v>
-      </c>
       <c r="I95">
-        <f t="shared" si="75"/>
+        <f t="shared" ref="I95" si="75">(2/3)*$B95*((13-E95)/12)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J95">
+        <f t="shared" ref="J95" si="76">(2/3)*$B95*((13-F95)/12)</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="J95">
-        <f t="shared" si="76"/>
-        <v>1</v>
-      </c>
       <c r="K95">
-        <f t="shared" si="77"/>
-        <v>2.166666666666667</v>
+        <f t="shared" ref="K95" si="77">I95+J95</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B96">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C96">
-        <v>140</v>
+        <v>36</v>
       </c>
       <c r="E96">
+        <v>4</v>
+      </c>
+      <c r="F96">
         <v>5</v>
       </c>
-      <c r="F96">
-        <v>3</v>
-      </c>
       <c r="I96">
-        <f t="shared" si="75"/>
-        <v>0.88888888888888884</v>
+        <f t="shared" ref="I96:I101" si="78">(2/3)*$B96*((13-E96)/12)</f>
+        <v>1.5</v>
       </c>
       <c r="J96">
-        <f t="shared" si="76"/>
-        <v>1.1111111111111112</v>
+        <f t="shared" ref="J96:J101" si="79">(2/3)*$B96*((13-F96)/12)</f>
+        <v>1.3333333333333333</v>
       </c>
       <c r="K96">
-        <f t="shared" si="77"/>
-        <v>2</v>
+        <f t="shared" ref="K96:K101" si="80">I96+J96</f>
+        <v>2.833333333333333</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C97">
         <v>60</v>
       </c>
       <c r="E97">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F97">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I97">
-        <f t="shared" si="75"/>
-        <v>0.88888888888888884</v>
+        <f t="shared" si="78"/>
+        <v>1.1666666666666667</v>
       </c>
       <c r="J97">
-        <f t="shared" si="76"/>
-        <v>1.1111111111111112</v>
+        <f t="shared" si="79"/>
+        <v>1</v>
       </c>
       <c r="K97">
-        <f t="shared" si="77"/>
-        <v>2</v>
+        <f t="shared" si="80"/>
+        <v>2.166666666666667</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B98">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E98">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F98">
         <v>3</v>
       </c>
       <c r="I98">
-        <f t="shared" si="75"/>
-        <v>0.83333333333333337</v>
+        <f t="shared" si="78"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J98">
-        <f t="shared" si="76"/>
-        <v>1.6666666666666667</v>
+        <f t="shared" si="79"/>
+        <v>1.1111111111111112</v>
       </c>
       <c r="K98">
-        <f t="shared" si="77"/>
-        <v>2.5</v>
+        <f t="shared" si="80"/>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99">
+        <v>60</v>
+      </c>
+      <c r="E99">
+        <v>5</v>
+      </c>
+      <c r="F99">
         <v>3</v>
       </c>
-      <c r="C99">
-        <v>36</v>
-      </c>
-      <c r="E99">
-        <v>4</v>
-      </c>
-      <c r="F99">
-        <v>6</v>
-      </c>
       <c r="I99">
-        <f t="shared" si="75"/>
-        <v>1.5</v>
+        <f t="shared" si="78"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J99">
-        <f t="shared" si="76"/>
-        <v>1.1666666666666667</v>
+        <f t="shared" si="79"/>
+        <v>1.1111111111111112</v>
       </c>
       <c r="K99">
-        <f t="shared" si="77"/>
-        <v>2.666666666666667</v>
+        <f t="shared" si="80"/>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>107</v>
+      </c>
+      <c r="B100">
+        <v>3</v>
+      </c>
+      <c r="C100">
+        <v>120</v>
+      </c>
+      <c r="E100">
+        <v>8</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="78"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="79"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K100">
+        <f t="shared" si="80"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>108</v>
+      </c>
+      <c r="B101">
+        <v>3</v>
+      </c>
+      <c r="C101">
+        <v>36</v>
+      </c>
+      <c r="E101">
+        <v>4</v>
+      </c>
+      <c r="F101">
+        <v>6</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="78"/>
+        <v>1.5</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="79"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="80"/>
+        <v>2.666666666666667</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>109</v>
       </c>
-      <c r="B100">
+      <c r="B102">
         <v>4</v>
       </c>
-      <c r="C100">
+      <c r="C102">
         <v>60</v>
       </c>
-      <c r="E100">
+      <c r="E102">
         <v>6</v>
       </c>
-      <c r="F100">
+      <c r="F102">
         <v>8</v>
       </c>
-      <c r="I100">
-        <f t="shared" ref="I100" si="78">(2/3)*$B100*((13-E100)/12)</f>
+      <c r="I102">
+        <f t="shared" ref="I102" si="81">(2/3)*$B102*((13-E102)/12)</f>
         <v>1.5555555555555556</v>
       </c>
-      <c r="J100">
-        <f t="shared" ref="J100" si="79">(2/3)*$B100*((13-F100)/12)</f>
+      <c r="J102">
+        <f t="shared" ref="J102" si="82">(2/3)*$B102*((13-F102)/12)</f>
         <v>1.1111111111111112</v>
       </c>
-      <c r="K100">
-        <f t="shared" ref="K100" si="80">I100+J100</f>
+      <c r="K102">
+        <f t="shared" ref="K102" si="83">I102+J102</f>
         <v>2.666666666666667</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>115</v>
+      </c>
+      <c r="E104">
+        <v>6</v>
+      </c>
+      <c r="F104">
+        <v>4</v>
+      </c>
+      <c r="I104">
+        <f>(5/6)*$B104*((13-E104)/12)</f>
+        <v>1.4583333333333335</v>
+      </c>
+      <c r="J104">
+        <f>(5/6)*$B104*((13-F104)/12)</f>
+        <v>1.875</v>
+      </c>
+      <c r="K104">
+        <f>I104+J104</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105">
+        <v>3</v>
+      </c>
+      <c r="C105">
+        <v>72</v>
+      </c>
+      <c r="E105">
+        <v>5</v>
+      </c>
+      <c r="F105">
+        <v>7</v>
+      </c>
+      <c r="I105">
+        <f t="shared" ref="I105:J111" si="84">(2/3)*$B105*((13-E105)/12)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="84"/>
+        <v>1</v>
+      </c>
+      <c r="K105">
+        <f>I105+J105</f>
+        <v>2.333333333333333</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>110</v>
+      </c>
+      <c r="B106">
+        <v>3</v>
+      </c>
+      <c r="C106">
+        <v>24</v>
+      </c>
+      <c r="E106">
+        <v>6</v>
+      </c>
+      <c r="F106">
+        <v>3</v>
+      </c>
+      <c r="I106">
+        <f t="shared" si="84"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="84"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K106">
+        <f>I106+J106</f>
+        <v>2.8333333333333335</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107">
+        <v>120</v>
+      </c>
+      <c r="E107">
+        <v>8</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="I107">
+        <f t="shared" si="84"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="84"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K107">
+        <f>I107+J107</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>111</v>
+      </c>
+      <c r="I108">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <f t="shared" ref="K108:K111" si="85">I108+J108</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I109">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="K109">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110">
+        <v>2</v>
+      </c>
+      <c r="C110">
+        <v>48</v>
+      </c>
+      <c r="E110">
+        <v>6</v>
+      </c>
+      <c r="F110">
+        <v>7</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="84"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="84"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="85"/>
+        <v>1.4444444444444444</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>48</v>
+      </c>
+      <c r="E111">
+        <v>8</v>
+      </c>
+      <c r="F111">
+        <v>2</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="84"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="84"/>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="K111">
+        <f t="shared" si="85"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>116</v>
+      </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <v>72</v>
+      </c>
+      <c r="E113">
+        <v>7</v>
+      </c>
+      <c r="F113">
+        <v>10</v>
+      </c>
+      <c r="I113">
+        <f t="shared" ref="I113:I115" si="86">(2/3)*$B113*((13-E113)/12)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J113">
+        <f t="shared" ref="J113:J115" si="87">(2/3)*$B113*((13-F113)/12)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K113">
+        <f t="shared" ref="K113:K115" si="88">I113+J113</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>117</v>
+      </c>
+      <c r="B114">
+        <v>2</v>
+      </c>
+      <c r="C114">
+        <v>48</v>
+      </c>
+      <c r="E114">
+        <v>10</v>
+      </c>
+      <c r="F114">
+        <v>5</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="86"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="87"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="K114">
+        <f t="shared" si="88"/>
+        <v>1.2222222222222221</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>118</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115">
+        <v>48</v>
+      </c>
+      <c r="E115">
+        <v>8</v>
+      </c>
+      <c r="F115">
+        <v>7</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="86"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J115">
+        <f t="shared" si="87"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K115">
+        <f t="shared" si="88"/>
+        <v>1.2222222222222223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Heavy points to be in line with Leman Russ
</commit_message>
<xml_diff>
--- a/Raw Data/weapons.xlsx
+++ b/Raw Data/weapons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Battlescribe\github\40klite\40klite\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F1951C-FE25-4C38-AFB8-AEE715188026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FD57F8-040A-4128-8F6D-F5D37F449FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="129">
   <si>
     <t>Weapon</t>
   </si>
@@ -399,6 +399,30 @@
   </si>
   <si>
     <t>Gauss Cannon</t>
+  </si>
+  <si>
+    <t>Better Movement</t>
+  </si>
+  <si>
+    <t>Worse WS</t>
+  </si>
+  <si>
+    <t>Worse A</t>
+  </si>
+  <si>
+    <t>Better Sv</t>
+  </si>
+  <si>
+    <t>No Lasgun</t>
+  </si>
+  <si>
+    <t>Double Tap</t>
+  </si>
+  <si>
+    <t>Is Heavy</t>
+  </si>
+  <si>
+    <t>Hull Weapon</t>
   </si>
 </sst>
 </file>
@@ -837,8 +861,8 @@
   <dimension ref="A1:V115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S85" sqref="P85:S101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3689,7 +3713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -3718,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>95</v>
       </c>
@@ -3747,7 +3771,7 @@
         <v>1.8333333333333335</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -3776,7 +3800,7 @@
         <v>1.8888888888888888</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -3805,7 +3829,12 @@
         <v>1.6666666666666665</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>97</v>
       </c>
@@ -3830,8 +3859,14 @@
         <f t="shared" ref="K87:K90" si="68">I87+J87</f>
         <v>2.333333333333333</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q87" t="s">
+        <v>121</v>
+      </c>
+      <c r="R87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>98</v>
       </c>
@@ -3856,8 +3891,14 @@
         <f t="shared" si="68"/>
         <v>1.5555555555555556</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q88" t="s">
+        <v>122</v>
+      </c>
+      <c r="R88">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>99</v>
       </c>
@@ -3882,8 +3923,14 @@
         <f t="shared" si="68"/>
         <v>2.4444444444444442</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q89" t="s">
+        <v>123</v>
+      </c>
+      <c r="R89">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>15</v>
       </c>
@@ -3908,8 +3955,22 @@
         <f t="shared" si="68"/>
         <v>0.61111111111111116</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q90" t="s">
+        <v>124</v>
+      </c>
+      <c r="R90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q91" t="s">
+        <v>125</v>
+      </c>
+      <c r="R91">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -3937,8 +3998,14 @@
         <f t="shared" ref="K92" si="71">I92+J92</f>
         <v>1.3333333333333333</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q92" t="s">
+        <v>16</v>
+      </c>
+      <c r="R92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -3966,8 +4033,22 @@
         <f t="shared" ref="K93" si="74">I93+J93</f>
         <v>0.77777777777777768</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q93" t="s">
+        <v>126</v>
+      </c>
+      <c r="R93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q94" t="s">
+        <v>127</v>
+      </c>
+      <c r="R94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -3995,8 +4076,14 @@
         <f t="shared" ref="K95" si="77">I95+J95</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q95" t="s">
+        <v>128</v>
+      </c>
+      <c r="R95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -4023,6 +4110,10 @@
       <c r="K96">
         <f t="shared" ref="K96:K101" si="80">I96+J96</f>
         <v>2.833333333333333</v>
+      </c>
+      <c r="R96">
+        <f>SUM(R86:R95)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Nerfed Russ weapons, fixed knight stuff
</commit_message>
<xml_diff>
--- a/Raw Data/weapons.xlsx
+++ b/Raw Data/weapons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Battlescribe\github\40klite\40klite\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FD57F8-040A-4128-8F6D-F5D37F449FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00639559-0EFB-47A7-9141-08D7DD50875A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -861,8 +861,8 @@
   <dimension ref="A1:V115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S85" sqref="P85:S101"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,26 +1244,25 @@
         <v>0</v>
       </c>
       <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
         <v>4</v>
       </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-      <c r="G11">
-        <f>SUM(D11:F11)/B11</f>
-        <v>4</v>
-      </c>
       <c r="I11">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" ref="I11" si="11">(2/3)*$B11*((13-E11)/12)</f>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J11">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" ref="J11" si="12">(2/3)*$B11*((13-F11)/12)</f>
+        <v>0.88888888888888884</v>
       </c>
       <c r="K11">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" ref="K11" si="13">I11+J11</f>
+        <v>1.7777777777777777</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1281,26 +1280,26 @@
         <v>-4</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <f>SUM(D12:F12)/B12</f>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="I12">
         <f t="shared" si="6"/>
-        <v>0.88888888888888884</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="J12">
         <f t="shared" si="7"/>
-        <v>0.77777777777777779</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K12">
         <f t="shared" si="8"/>
-        <v>1.6666666666666665</v>
+        <v>1.4444444444444444</v>
       </c>
       <c r="M12">
         <f>3.5*(5/6)*2</f>
@@ -1326,30 +1325,30 @@
         <v>72</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:D17" si="11">(24-C13)/12</f>
+        <f t="shared" ref="D13:D17" si="14">(24-C13)/12</f>
         <v>-4</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G17" si="12">SUM(D13:F13)/B13</f>
-        <v>3.5</v>
+        <f t="shared" ref="G13:G17" si="15">SUM(D13:F13)/B13</f>
+        <v>4.5</v>
       </c>
       <c r="I13">
         <f t="shared" si="6"/>
-        <v>0.44444444444444442</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J13">
         <f t="shared" si="7"/>
-        <v>1.2222222222222221</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="K13">
         <f t="shared" si="8"/>
-        <v>1.6666666666666665</v>
+        <v>1.4444444444444444</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1363,30 +1362,30 @@
         <v>24</v>
       </c>
       <c r="D14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14">
-        <f t="shared" si="12"/>
-        <v>4.666666666666667</v>
+        <f t="shared" si="15"/>
+        <v>5.333333333333333</v>
       </c>
       <c r="I14">
         <f t="shared" si="6"/>
-        <v>1.3333333333333333</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="J14">
         <f t="shared" si="7"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="K14">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1400,18 +1399,18 @@
         <v>36</v>
       </c>
       <c r="D15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-1</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="15"/>
         <v>5</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="12"/>
-        <v>4</v>
       </c>
       <c r="I15">
         <f t="shared" si="6"/>
@@ -1419,11 +1418,11 @@
       </c>
       <c r="J15">
         <f t="shared" si="7"/>
-        <v>0.88888888888888884</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K15">
         <f t="shared" si="8"/>
-        <v>1.8888888888888888</v>
+        <v>1.6666666666666665</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1437,30 +1436,30 @@
         <v>48</v>
       </c>
       <c r="D16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-2</v>
       </c>
       <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="15"/>
         <v>5</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="12"/>
-        <v>4</v>
       </c>
       <c r="I16">
         <f t="shared" si="6"/>
-        <v>0.88888888888888884</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="J16">
         <f t="shared" si="7"/>
-        <v>0.88888888888888884</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="K16">
         <f t="shared" si="8"/>
-        <v>1.7777777777777777</v>
+        <v>1.5555555555555556</v>
       </c>
       <c r="P16">
         <f>8*(1/3)*2</f>
@@ -1478,18 +1477,18 @@
         <v>36</v>
       </c>
       <c r="D17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-1</v>
       </c>
       <c r="E17">
         <v>5</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G17">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="15"/>
+        <v>5</v>
       </c>
       <c r="I17">
         <f t="shared" si="6"/>
@@ -1497,11 +1496,11 @@
       </c>
       <c r="J17">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="K17">
         <f t="shared" si="8"/>
-        <v>1.8888888888888888</v>
+        <v>1.6666666666666665</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1515,33 +1514,33 @@
         <v>48</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:D23" si="13">(24-C18)/12</f>
+        <f t="shared" ref="D18:D23" si="16">(24-C18)/12</f>
         <v>-2</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F18">
         <v>11</v>
       </c>
       <c r="G18">
         <f>SUM(D18:F18)/B18</f>
-        <v>4.333333333333333</v>
+        <v>5</v>
       </c>
       <c r="H18" t="s">
         <v>57</v>
       </c>
       <c r="I18">
-        <f t="shared" ref="I18:J20" si="14">(2/3)*$B18*((13-E18)/12)</f>
+        <f t="shared" ref="I18:J20" si="17">(2/3)*$B18*((13-E18)/12)</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="17"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18:K20" si="18">I18+J18</f>
         <v>1.5</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="14"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K18">
-        <f t="shared" ref="K18:K20" si="15">I18+J18</f>
-        <v>1.8333333333333333</v>
       </c>
       <c r="M18" t="s">
         <v>76</v>
@@ -1582,33 +1581,33 @@
         <v>72</v>
       </c>
       <c r="D19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-4</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G19">
         <f>SUM(D19:F19)/B19</f>
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="H19" t="s">
         <v>57</v>
       </c>
       <c r="I19">
-        <f t="shared" si="14"/>
-        <v>0.88888888888888884</v>
+        <f t="shared" si="17"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J19">
-        <f t="shared" si="14"/>
-        <v>0.77777777777777779</v>
+        <f t="shared" si="17"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K19">
-        <f t="shared" si="15"/>
-        <v>1.6666666666666665</v>
+        <f t="shared" si="18"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="L19">
         <f>SUM(M19:U19)</f>
@@ -1650,33 +1649,33 @@
         <v>72</v>
       </c>
       <c r="D20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-4</v>
       </c>
       <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
         <v>6</v>
-      </c>
-      <c r="F20">
-        <v>5</v>
       </c>
       <c r="G20">
         <f>SUM(D20:F20)/B20</f>
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="H20" t="s">
         <v>57</v>
       </c>
       <c r="I20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="17"/>
         <v>0.77777777777777779</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="14"/>
-        <v>0.88888888888888884</v>
-      </c>
       <c r="K20">
-        <f t="shared" si="15"/>
-        <v>1.6666666666666665</v>
+        <f t="shared" si="18"/>
+        <v>1.3333333333333335</v>
       </c>
       <c r="L20">
         <f>SUM(M20:U20)</f>
@@ -1712,7 +1711,7 @@
         <v>36</v>
       </c>
       <c r="D21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-1</v>
       </c>
     </row>
@@ -1727,7 +1726,7 @@
         <v>36</v>
       </c>
       <c r="D22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-1</v>
       </c>
       <c r="E22">
@@ -1737,15 +1736,15 @@
         <v>5</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22" si="16">(2/3)*$B22*((13-E22)/12)</f>
+        <f t="shared" ref="I22" si="19">(2/3)*$B22*((13-E22)/12)</f>
         <v>0.5</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22" si="17">(2/3)*$B22*((13-F22)/12)</f>
+        <f t="shared" ref="J22" si="20">(2/3)*$B22*((13-F22)/12)</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22" si="18">I22+J22</f>
+        <f t="shared" ref="K22" si="21">I22+J22</f>
         <v>1.8333333333333333</v>
       </c>
     </row>
@@ -1760,7 +1759,7 @@
         <v>36</v>
       </c>
       <c r="D23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-1</v>
       </c>
       <c r="E23">
@@ -1770,15 +1769,15 @@
         <v>8</v>
       </c>
       <c r="I23">
-        <f t="shared" ref="I23" si="19">(2/3)*$B23*((13-E23)/12)</f>
+        <f t="shared" ref="I23" si="22">(2/3)*$B23*((13-E23)/12)</f>
         <v>1</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23" si="20">(2/3)*$B23*((13-F23)/12)</f>
+        <f t="shared" ref="J23" si="23">(2/3)*$B23*((13-F23)/12)</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="K23" si="21">I23+J23</f>
+        <f t="shared" ref="K23" si="24">I23+J23</f>
         <v>1.8333333333333335</v>
       </c>
     </row>
@@ -1837,15 +1836,15 @@
         <v>17</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I36" si="22">(2/3)*$B25*((13-E25)/12)</f>
+        <f t="shared" ref="I25:I36" si="25">(2/3)*$B25*((13-E25)/12)</f>
         <v>0.27777777777777779</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:J36" si="23">(2/3)*$B25*((13-F25)/12)</f>
+        <f t="shared" ref="J25:J36" si="26">(2/3)*$B25*((13-F25)/12)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K36" si="24">I25+J25</f>
+        <f t="shared" ref="K25:K36" si="27">I25+J25</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="L25">
@@ -1896,15 +1895,15 @@
         <v>28</v>
       </c>
       <c r="I26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="K26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0.5</v>
       </c>
       <c r="L26">
@@ -1935,15 +1934,15 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I27">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="J27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="M27">
@@ -1970,7 +1969,7 @@
         <v>24</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:D36" si="25">(24-C28)/12</f>
+        <f t="shared" ref="D28:D36" si="28">(24-C28)/12</f>
         <v>0</v>
       </c>
       <c r="E28">
@@ -1980,19 +1979,19 @@
         <v>11</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:G36" si="26">SUM(D28:F28)/B28</f>
+        <f t="shared" ref="G28:G36" si="29">SUM(D28:F28)/B28</f>
         <v>6</v>
       </c>
       <c r="I28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="J28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="M28">
@@ -2022,7 +2021,7 @@
         <v>12</v>
       </c>
       <c r="D29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="E29">
@@ -2032,19 +2031,19 @@
         <v>8</v>
       </c>
       <c r="G29">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="25"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="26"/>
-        <v>7</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="22"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="23"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="K29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>1.4444444444444444</v>
       </c>
       <c r="O29">
@@ -2068,7 +2067,7 @@
         <v>24</v>
       </c>
       <c r="D30">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="E30">
@@ -2078,19 +2077,19 @@
         <v>6</v>
       </c>
       <c r="G30">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="25"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="26"/>
-        <v>7</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="22"/>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="23"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="K30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>1.3333333333333335</v>
       </c>
     </row>
@@ -2105,7 +2104,7 @@
         <v>12</v>
       </c>
       <c r="D31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="E31">
@@ -2115,19 +2114,19 @@
         <v>8</v>
       </c>
       <c r="G31">
+        <f t="shared" si="29"/>
+        <v>14</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="25"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="26"/>
-        <v>14</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="22"/>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="23"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
@@ -2142,7 +2141,7 @@
         <v>24</v>
       </c>
       <c r="D32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="E32">
@@ -2152,19 +2151,19 @@
         <v>9</v>
       </c>
       <c r="G32">
+        <f t="shared" si="29"/>
+        <v>14</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="25"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J32">
         <f t="shared" si="26"/>
-        <v>14</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="22"/>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="23"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="K32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -2179,29 +2178,29 @@
         <v>24</v>
       </c>
       <c r="D33">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>7</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="29"/>
+        <v>14</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>7</v>
-      </c>
-      <c r="F33">
-        <v>7</v>
-      </c>
-      <c r="G33">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J33">
         <f t="shared" si="26"/>
-        <v>14</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="22"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J33">
-        <f t="shared" si="23"/>
-        <v>0.33333333333333331</v>
-      </c>
       <c r="K33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -2216,7 +2215,7 @@
         <v>36</v>
       </c>
       <c r="D34">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>-1</v>
       </c>
       <c r="E34">
@@ -2226,19 +2225,19 @@
         <v>10</v>
       </c>
       <c r="G34">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="25"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J34">
         <f t="shared" si="26"/>
-        <v>8</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="22"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="23"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K34">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
     </row>
@@ -2253,7 +2252,7 @@
         <v>72</v>
       </c>
       <c r="D35">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>-4</v>
       </c>
       <c r="E35">
@@ -2263,19 +2262,19 @@
         <v>6</v>
       </c>
       <c r="G35">
+        <f t="shared" si="29"/>
+        <v>6.5</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="25"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J35">
         <f t="shared" si="26"/>
-        <v>6.5</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="22"/>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="23"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="K35">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
     </row>
@@ -2290,7 +2289,7 @@
         <v>24</v>
       </c>
       <c r="D36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="E36">
@@ -2300,19 +2299,19 @@
         <v>10</v>
       </c>
       <c r="G36">
+        <f t="shared" si="29"/>
+        <v>17</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="25"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J36">
         <f t="shared" si="26"/>
-        <v>17</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="22"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="23"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="K36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2327,7 +2326,7 @@
         <v>36</v>
       </c>
       <c r="D38">
-        <f t="shared" ref="D38:D43" si="27">(24-C38)/12</f>
+        <f t="shared" ref="D38:D43" si="30">(24-C38)/12</f>
         <v>-1</v>
       </c>
       <c r="E38">
@@ -2337,19 +2336,19 @@
         <v>10</v>
       </c>
       <c r="G38">
-        <f t="shared" ref="G38:G53" si="28">SUM(D38:F38)/B38</f>
+        <f t="shared" ref="G38:G53" si="31">SUM(D38:F38)/B38</f>
         <v>14</v>
       </c>
       <c r="I38">
-        <f t="shared" ref="I38:I53" si="29">(2/3)*$B38*((13-E38)/12)</f>
+        <f t="shared" ref="I38:I53" si="32">(2/3)*$B38*((13-E38)/12)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J38:J53" si="30">(2/3)*$B38*((13-F38)/12)</f>
+        <f t="shared" ref="J38:J53" si="33">(2/3)*$B38*((13-F38)/12)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="K38">
-        <f t="shared" ref="K38:K53" si="31">I38+J38</f>
+        <f t="shared" ref="K38:K53" si="34">I38+J38</f>
         <v>0.61111111111111105</v>
       </c>
     </row>
@@ -2364,7 +2363,7 @@
         <v>24</v>
       </c>
       <c r="D39">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="E39">
@@ -2374,19 +2373,19 @@
         <v>8</v>
       </c>
       <c r="G39">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I39">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K39">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
@@ -2401,7 +2400,7 @@
         <v>36</v>
       </c>
       <c r="D40">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>-1</v>
       </c>
       <c r="E40">
@@ -2411,19 +2410,19 @@
         <v>7</v>
       </c>
       <c r="G40">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I40">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K40">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -2438,7 +2437,7 @@
         <v>36</v>
       </c>
       <c r="D41">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>-1</v>
       </c>
       <c r="E41">
@@ -2448,19 +2447,19 @@
         <v>4</v>
       </c>
       <c r="G41">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I41">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="K41">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="T41" s="2"/>
@@ -2476,7 +2475,7 @@
         <v>48</v>
       </c>
       <c r="D42">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>-2</v>
       </c>
       <c r="E42">
@@ -2486,19 +2485,19 @@
         <v>8</v>
       </c>
       <c r="G42">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I42">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K42">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.61111111111111116</v>
       </c>
     </row>
@@ -2513,7 +2512,7 @@
         <v>12</v>
       </c>
       <c r="D43">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="E43">
@@ -2523,37 +2522,37 @@
         <v>10</v>
       </c>
       <c r="G43">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
       <c r="I43">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K43">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G44" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I44">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="K44">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -2568,7 +2567,7 @@
         <v>36</v>
       </c>
       <c r="D45">
-        <f t="shared" ref="D45:D53" si="32">(24-C45)/12</f>
+        <f t="shared" ref="D45:D53" si="35">(24-C45)/12</f>
         <v>-1</v>
       </c>
       <c r="E45">
@@ -2578,19 +2577,19 @@
         <v>9</v>
       </c>
       <c r="G45">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="K45">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="M45">
@@ -2613,7 +2612,7 @@
         <v>36</v>
       </c>
       <c r="D46">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>-1</v>
       </c>
       <c r="E46">
@@ -2623,19 +2622,19 @@
         <v>8</v>
       </c>
       <c r="G46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I46">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.3888888888888889</v>
       </c>
       <c r="J46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.66666666666666674</v>
       </c>
     </row>
@@ -2650,7 +2649,7 @@
         <v>24</v>
       </c>
       <c r="D47">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="E47">
@@ -2660,19 +2659,19 @@
         <v>8</v>
       </c>
       <c r="G47">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I47">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
@@ -2687,7 +2686,7 @@
         <v>48</v>
       </c>
       <c r="D48">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>-2</v>
       </c>
       <c r="E48">
@@ -2697,19 +2696,19 @@
         <v>8</v>
       </c>
       <c r="G48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.61111111111111116</v>
       </c>
     </row>
@@ -2724,7 +2723,7 @@
         <v>48</v>
       </c>
       <c r="D49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>-2</v>
       </c>
       <c r="E49">
@@ -2734,19 +2733,19 @@
         <v>7</v>
       </c>
       <c r="G49">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I49">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="J49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K49">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.61111111111111116</v>
       </c>
     </row>
@@ -2761,7 +2760,7 @@
         <v>24</v>
       </c>
       <c r="D50">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="E50">
@@ -2771,19 +2770,19 @@
         <v>4</v>
       </c>
       <c r="G50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="J50">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="K50">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
@@ -2798,29 +2797,29 @@
         <v>36</v>
       </c>
       <c r="D51">
+        <f t="shared" si="35"/>
+        <v>-1</v>
+      </c>
+      <c r="E51">
+        <v>7</v>
+      </c>
+      <c r="F51">
+        <v>7</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="31"/>
+        <v>13</v>
+      </c>
+      <c r="I51">
         <f t="shared" si="32"/>
-        <v>-1</v>
-      </c>
-      <c r="E51">
-        <v>7</v>
-      </c>
-      <c r="F51">
-        <v>7</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="28"/>
-        <v>13</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="29"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J51">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K51">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -2835,7 +2834,7 @@
         <v>48</v>
       </c>
       <c r="D52">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>-2</v>
       </c>
       <c r="E52">
@@ -2845,19 +2844,19 @@
         <v>5</v>
       </c>
       <c r="G52">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="I52">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J52">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="K52">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.61111111111111105</v>
       </c>
       <c r="M52">
@@ -2876,7 +2875,7 @@
         <v>12</v>
       </c>
       <c r="D53">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="E53">
@@ -2886,22 +2885,22 @@
         <v>8</v>
       </c>
       <c r="G53">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>14</v>
       </c>
       <c r="H53" t="s">
         <v>22</v>
       </c>
       <c r="I53">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K53">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
@@ -2916,7 +2915,7 @@
         <v>48</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55:D67" si="33">(24-C55)/12</f>
+        <f t="shared" ref="D55:D67" si="36">(24-C55)/12</f>
         <v>-2</v>
       </c>
       <c r="E55">
@@ -2926,19 +2925,19 @@
         <v>7</v>
       </c>
       <c r="G55">
-        <f t="shared" ref="G55:G61" si="34">SUM(D55:F55)/B55</f>
+        <f t="shared" ref="G55:G61" si="37">SUM(D55:F55)/B55</f>
         <v>6.5</v>
       </c>
       <c r="I55">
-        <f t="shared" ref="I55:J63" si="35">(2/3)*$B55*((13-E55)/12)</f>
+        <f t="shared" ref="I55:J63" si="38">(2/3)*$B55*((13-E55)/12)</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="J55">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="K55">
-        <f t="shared" ref="K55:K63" si="36">I55+J55</f>
+        <f t="shared" ref="K55:K63" si="39">I55+J55</f>
         <v>1.2222222222222223</v>
       </c>
     </row>
@@ -2953,7 +2952,7 @@
         <v>48</v>
       </c>
       <c r="D56">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>-2</v>
       </c>
       <c r="E56">
@@ -2963,19 +2962,19 @@
         <v>8</v>
       </c>
       <c r="G56">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>13</v>
       </c>
       <c r="I56">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J56">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K56">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.61111111111111116</v>
       </c>
     </row>
@@ -2990,7 +2989,7 @@
         <v>24</v>
       </c>
       <c r="D57">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E57">
@@ -3000,19 +2999,19 @@
         <v>8</v>
       </c>
       <c r="G57">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>6.5</v>
       </c>
       <c r="I57">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="J57">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="K57">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1.4444444444444444</v>
       </c>
     </row>
@@ -3027,7 +3026,7 @@
         <v>36</v>
       </c>
       <c r="D58">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>-1</v>
       </c>
       <c r="E58">
@@ -3037,19 +3036,19 @@
         <v>8</v>
       </c>
       <c r="G58">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>6.5</v>
       </c>
       <c r="I58">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="J58">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="K58">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1.3333333333333335</v>
       </c>
     </row>
@@ -3064,7 +3063,7 @@
         <v>24</v>
       </c>
       <c r="D59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E59">
@@ -3074,19 +3073,19 @@
         <v>4</v>
       </c>
       <c r="G59">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>13</v>
       </c>
       <c r="I59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="J59">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.5</v>
       </c>
       <c r="K59">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.72222222222222221</v>
       </c>
     </row>
@@ -3101,7 +3100,7 @@
         <v>36</v>
       </c>
       <c r="D60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>-1</v>
       </c>
       <c r="E60">
@@ -3111,19 +3110,19 @@
         <v>7</v>
       </c>
       <c r="G60">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>13</v>
       </c>
       <c r="I60">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J60">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K60">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -3138,7 +3137,7 @@
         <v>48</v>
       </c>
       <c r="D61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>-2</v>
       </c>
       <c r="E61">
@@ -3148,19 +3147,19 @@
         <v>5</v>
       </c>
       <c r="G61">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>6.5</v>
       </c>
       <c r="I61">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J61">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="K61">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1.2222222222222221</v>
       </c>
       <c r="O61">
@@ -3179,7 +3178,7 @@
         <v>12</v>
       </c>
       <c r="D62">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="E62">
@@ -3189,22 +3188,22 @@
         <v>8</v>
       </c>
       <c r="G62">
-        <f t="shared" ref="G62:G66" si="37">SUM(D62:F62)/B62</f>
+        <f t="shared" ref="G62:G66" si="40">SUM(D62:F62)/B62</f>
         <v>7</v>
       </c>
       <c r="H62" t="s">
         <v>22</v>
       </c>
       <c r="I62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="J62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="K62">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1.4444444444444444</v>
       </c>
     </row>
@@ -3219,7 +3218,7 @@
         <v>48</v>
       </c>
       <c r="D63">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>-2</v>
       </c>
       <c r="E63">
@@ -3229,19 +3228,19 @@
         <v>5</v>
       </c>
       <c r="G63">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>6.5</v>
       </c>
       <c r="I63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="K63">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1.2222222222222221</v>
       </c>
     </row>
@@ -3256,7 +3255,7 @@
         <v>18</v>
       </c>
       <c r="D64">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0.5</v>
       </c>
       <c r="E64">
@@ -3266,19 +3265,19 @@
         <v>11</v>
       </c>
       <c r="G64">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>4.375</v>
       </c>
       <c r="I64">
-        <f t="shared" ref="I64" si="38">(2/3)*$B64*((13-E64)/12)</f>
+        <f t="shared" ref="I64" si="41">(2/3)*$B64*((13-E64)/12)</f>
         <v>1.5555555555555556</v>
       </c>
       <c r="J64">
-        <f t="shared" ref="J64" si="39">(2/3)*$B64*((13-F64)/12)</f>
+        <f t="shared" ref="J64" si="42">(2/3)*$B64*((13-F64)/12)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="K64">
-        <f t="shared" ref="K64" si="40">I64+J64</f>
+        <f t="shared" ref="K64" si="43">I64+J64</f>
         <v>2</v>
       </c>
     </row>
@@ -3293,7 +3292,7 @@
         <v>18</v>
       </c>
       <c r="D65">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0.5</v>
       </c>
       <c r="E65">
@@ -3303,19 +3302,19 @@
         <v>8</v>
       </c>
       <c r="G65">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>7.25</v>
       </c>
       <c r="I65">
-        <f t="shared" ref="I65:I70" si="41">(2/3)*$B65*((13-E65)/12)</f>
+        <f t="shared" ref="I65:I70" si="44">(2/3)*$B65*((13-E65)/12)</f>
         <v>0.77777777777777779</v>
       </c>
       <c r="J65">
-        <f t="shared" ref="J65:J70" si="42">(2/3)*$B65*((13-F65)/12)</f>
+        <f t="shared" ref="J65:J70" si="45">(2/3)*$B65*((13-F65)/12)</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="K65">
-        <f t="shared" ref="K65:K70" si="43">I65+J65</f>
+        <f t="shared" ref="K65:K70" si="46">I65+J65</f>
         <v>1.3333333333333335</v>
       </c>
       <c r="S65">
@@ -3342,7 +3341,7 @@
         <v>30</v>
       </c>
       <c r="D66">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>-0.5</v>
       </c>
       <c r="E66">
@@ -3352,19 +3351,19 @@
         <v>8</v>
       </c>
       <c r="G66">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>6.75</v>
       </c>
       <c r="I66">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="J66">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="K66">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>1.3333333333333335</v>
       </c>
     </row>
@@ -3379,7 +3378,7 @@
         <v>24</v>
       </c>
       <c r="D67">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E67">
@@ -3389,15 +3388,15 @@
         <v>6</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67" si="44">(2/3)*$B67*((13-E67)/12)</f>
+        <f t="shared" ref="I67" si="47">(2/3)*$B67*((13-E67)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67" si="45">(2/3)*$B67*((13-F67)/12)</f>
+        <f t="shared" ref="J67" si="48">(2/3)*$B67*((13-F67)/12)</f>
         <v>0.77777777777777779</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67" si="46">I67+J67</f>
+        <f t="shared" ref="K67" si="49">I67+J67</f>
         <v>1.4444444444444444</v>
       </c>
     </row>
@@ -3409,7 +3408,7 @@
         <v>36</v>
       </c>
       <c r="D68">
-        <f t="shared" ref="D68:D70" si="47">(24-C68)/12</f>
+        <f t="shared" ref="D68:D70" si="50">(24-C68)/12</f>
         <v>-1</v>
       </c>
       <c r="E68">
@@ -3426,15 +3425,15 @@
         <v>22</v>
       </c>
       <c r="I68">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="J68">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="K68">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>1.4444444444444444</v>
       </c>
       <c r="M68" t="s">
@@ -3452,7 +3451,7 @@
         <v>36</v>
       </c>
       <c r="D69">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>-1</v>
       </c>
       <c r="E69">
@@ -3466,15 +3465,15 @@
         <v>6.5</v>
       </c>
       <c r="I69">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J69">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="K69">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="L69" t="s">
@@ -3492,7 +3491,7 @@
         <v>24</v>
       </c>
       <c r="D70">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="E70">
@@ -3506,15 +3505,15 @@
         <v>6</v>
       </c>
       <c r="I70">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J70">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="K70">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>1.5555555555555554</v>
       </c>
       <c r="L70">
@@ -3538,15 +3537,15 @@
         <v>8</v>
       </c>
       <c r="I72">
-        <f t="shared" ref="I72" si="48">(2/3)*$B72*((13-E72)/12)</f>
+        <f t="shared" ref="I72" si="51">(2/3)*$B72*((13-E72)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J72">
-        <f t="shared" ref="J72" si="49">(2/3)*$B72*((13-F72)/12)</f>
+        <f t="shared" ref="J72" si="52">(2/3)*$B72*((13-F72)/12)</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="K72">
-        <f t="shared" ref="K72" si="50">I72+J72</f>
+        <f t="shared" ref="K72" si="53">I72+J72</f>
         <v>1.2222222222222223</v>
       </c>
     </row>
@@ -3567,15 +3566,15 @@
         <v>12</v>
       </c>
       <c r="I73">
-        <f t="shared" ref="I73:I74" si="51">(2/3)*$B73*((13-E73)/12)</f>
+        <f t="shared" ref="I73:I74" si="54">(2/3)*$B73*((13-E73)/12)</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J74" si="52">(2/3)*$B73*((13-F73)/12)</f>
+        <f t="shared" ref="J73:J74" si="55">(2/3)*$B73*((13-F73)/12)</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="K73">
-        <f t="shared" ref="K73:K74" si="53">I73+J73</f>
+        <f t="shared" ref="K73:K74" si="56">I73+J73</f>
         <v>1.5555555555555554</v>
       </c>
     </row>
@@ -3596,15 +3595,15 @@
         <v>6</v>
       </c>
       <c r="I74">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J74">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="K74">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>1.2222222222222223</v>
       </c>
     </row>
@@ -3643,15 +3642,15 @@
         <v>10</v>
       </c>
       <c r="I77">
-        <f t="shared" ref="I77" si="54">(2/3)*$B77*((13-E77)/12)</f>
+        <f t="shared" ref="I77" si="57">(2/3)*$B77*((13-E77)/12)</f>
         <v>0.27777777777777779</v>
       </c>
       <c r="J77">
-        <f t="shared" ref="J77" si="55">(2/3)*$B77*((13-F77)/12)</f>
+        <f t="shared" ref="J77" si="58">(2/3)*$B77*((13-F77)/12)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="K77">
-        <f t="shared" ref="K77" si="56">I77+J77</f>
+        <f t="shared" ref="K77" si="59">I77+J77</f>
         <v>0.44444444444444442</v>
       </c>
     </row>
@@ -3672,15 +3671,15 @@
         <v>11</v>
       </c>
       <c r="I78">
-        <f t="shared" ref="I78" si="57">(2/3)*$B78*((13-E78)/12)</f>
+        <f t="shared" ref="I78" si="60">(2/3)*$B78*((13-E78)/12)</f>
         <v>0.3888888888888889</v>
       </c>
       <c r="J78">
-        <f t="shared" ref="J78" si="58">(2/3)*$B78*((13-F78)/12)</f>
+        <f t="shared" ref="J78" si="61">(2/3)*$B78*((13-F78)/12)</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="K78">
-        <f t="shared" ref="K78" si="59">I78+J78</f>
+        <f t="shared" ref="K78" si="62">I78+J78</f>
         <v>0.5</v>
       </c>
     </row>
@@ -3701,15 +3700,15 @@
         <v>10</v>
       </c>
       <c r="I80">
-        <f t="shared" ref="I80:I81" si="60">(2/3)*$B80*((13-E80)/12)</f>
+        <f t="shared" ref="I80:I81" si="63">(2/3)*$B80*((13-E80)/12)</f>
         <v>1.5</v>
       </c>
       <c r="J80">
-        <f t="shared" ref="J80:J81" si="61">(2/3)*$B80*((13-F80)/12)</f>
+        <f t="shared" ref="J80:J81" si="64">(2/3)*$B80*((13-F80)/12)</f>
         <v>0.5</v>
       </c>
       <c r="K80">
-        <f t="shared" ref="K80:K81" si="62">I80+J80</f>
+        <f t="shared" ref="K80:K81" si="65">I80+J80</f>
         <v>2</v>
       </c>
     </row>
@@ -3730,15 +3729,15 @@
         <v>7</v>
       </c>
       <c r="I81">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="J81">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="K81">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>2</v>
       </c>
     </row>
@@ -3759,15 +3758,15 @@
         <v>9</v>
       </c>
       <c r="I83">
-        <f t="shared" ref="I83:I85" si="63">(2/3)*$B83*((13-E83)/12)</f>
+        <f t="shared" ref="I83:I85" si="66">(2/3)*$B83*((13-E83)/12)</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J85" si="64">(2/3)*$B83*((13-F83)/12)</f>
+        <f t="shared" ref="J83:J85" si="67">(2/3)*$B83*((13-F83)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="K83">
-        <f t="shared" ref="K83:K85" si="65">I83+J83</f>
+        <f t="shared" ref="K83:K85" si="68">I83+J83</f>
         <v>1.8333333333333335</v>
       </c>
     </row>
@@ -3788,15 +3787,15 @@
         <v>5</v>
       </c>
       <c r="I84">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="J84">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="K84">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>1.8888888888888888</v>
       </c>
     </row>
@@ -3817,15 +3816,15 @@
         <v>5</v>
       </c>
       <c r="I85">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J85">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="K85">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>1.6666666666666665</v>
       </c>
     </row>
@@ -3848,15 +3847,15 @@
         <v>7</v>
       </c>
       <c r="I87">
-        <f t="shared" ref="I87:I90" si="66">(2/3)*$B87*((13-E87)/12)</f>
+        <f t="shared" ref="I87:I90" si="69">(2/3)*$B87*((13-E87)/12)</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="J87">
-        <f t="shared" ref="J87:J90" si="67">(2/3)*$B87*((13-F87)/12)</f>
+        <f t="shared" ref="J87:J90" si="70">(2/3)*$B87*((13-F87)/12)</f>
         <v>1</v>
       </c>
       <c r="K87">
-        <f t="shared" ref="K87:K90" si="68">I87+J87</f>
+        <f t="shared" ref="K87:K90" si="71">I87+J87</f>
         <v>2.333333333333333</v>
       </c>
       <c r="Q87" t="s">
@@ -3880,15 +3879,15 @@
         <v>4</v>
       </c>
       <c r="I88">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="J88">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="K88">
-        <f t="shared" si="68"/>
+        <f t="shared" si="71"/>
         <v>1.5555555555555556</v>
       </c>
       <c r="Q88" t="s">
@@ -3912,15 +3911,15 @@
         <v>10</v>
       </c>
       <c r="I89">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>1.7777777777777777</v>
       </c>
       <c r="J89">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="K89">
-        <f t="shared" si="68"/>
+        <f t="shared" si="71"/>
         <v>2.4444444444444442</v>
       </c>
       <c r="Q89" t="s">
@@ -3944,15 +3943,15 @@
         <v>8</v>
       </c>
       <c r="I90">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J90">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="K90">
-        <f t="shared" si="68"/>
+        <f t="shared" si="71"/>
         <v>0.61111111111111116</v>
       </c>
       <c r="Q90" t="s">
@@ -3987,15 +3986,15 @@
         <v>7</v>
       </c>
       <c r="I92">
-        <f t="shared" ref="I92" si="69">(2/3)*$B92*((13-E92)/12)</f>
+        <f t="shared" ref="I92" si="72">(2/3)*$B92*((13-E92)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J92">
-        <f t="shared" ref="J92" si="70">(2/3)*$B92*((13-F92)/12)</f>
+        <f t="shared" ref="J92" si="73">(2/3)*$B92*((13-F92)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="K92">
-        <f t="shared" ref="K92" si="71">I92+J92</f>
+        <f t="shared" ref="K92" si="74">I92+J92</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="Q92" t="s">
@@ -4022,15 +4021,15 @@
         <v>12</v>
       </c>
       <c r="I93">
-        <f t="shared" ref="I93" si="72">(2/3)*$B93*((13-E93)/12)</f>
+        <f t="shared" ref="I93" si="75">(2/3)*$B93*((13-E93)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J93">
-        <f t="shared" ref="J93" si="73">(2/3)*$B93*((13-F93)/12)</f>
+        <f t="shared" ref="J93" si="76">(2/3)*$B93*((13-F93)/12)</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="K93">
-        <f t="shared" ref="K93" si="74">I93+J93</f>
+        <f t="shared" ref="K93" si="77">I93+J93</f>
         <v>0.77777777777777768</v>
       </c>
       <c r="Q93" t="s">
@@ -4065,15 +4064,15 @@
         <v>6</v>
       </c>
       <c r="I95">
-        <f t="shared" ref="I95" si="75">(2/3)*$B95*((13-E95)/12)</f>
+        <f t="shared" ref="I95" si="78">(2/3)*$B95*((13-E95)/12)</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="J95">
-        <f t="shared" ref="J95" si="76">(2/3)*$B95*((13-F95)/12)</f>
+        <f t="shared" ref="J95" si="79">(2/3)*$B95*((13-F95)/12)</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="K95">
-        <f t="shared" ref="K95" si="77">I95+J95</f>
+        <f t="shared" ref="K95" si="80">I95+J95</f>
         <v>2.5</v>
       </c>
       <c r="Q95" t="s">
@@ -4100,15 +4099,15 @@
         <v>5</v>
       </c>
       <c r="I96">
-        <f t="shared" ref="I96:I101" si="78">(2/3)*$B96*((13-E96)/12)</f>
+        <f t="shared" ref="I96:I101" si="81">(2/3)*$B96*((13-E96)/12)</f>
         <v>1.5</v>
       </c>
       <c r="J96">
-        <f t="shared" ref="J96:J101" si="79">(2/3)*$B96*((13-F96)/12)</f>
+        <f t="shared" ref="J96:J101" si="82">(2/3)*$B96*((13-F96)/12)</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="K96">
-        <f t="shared" ref="K96:K101" si="80">I96+J96</f>
+        <f t="shared" ref="K96:K101" si="83">I96+J96</f>
         <v>2.833333333333333</v>
       </c>
       <c r="R96">
@@ -4133,15 +4132,15 @@
         <v>7</v>
       </c>
       <c r="I97">
-        <f t="shared" si="78"/>
+        <f t="shared" si="81"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="J97">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>1</v>
       </c>
       <c r="K97">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>2.166666666666667</v>
       </c>
     </row>
@@ -4162,15 +4161,15 @@
         <v>3</v>
       </c>
       <c r="I98">
-        <f t="shared" si="78"/>
+        <f t="shared" si="81"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="J98">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>1.1111111111111112</v>
       </c>
       <c r="K98">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>2</v>
       </c>
     </row>
@@ -4191,15 +4190,15 @@
         <v>3</v>
       </c>
       <c r="I99">
-        <f t="shared" si="78"/>
+        <f t="shared" si="81"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="J99">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>1.1111111111111112</v>
       </c>
       <c r="K99">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>2</v>
       </c>
     </row>
@@ -4220,15 +4219,15 @@
         <v>3</v>
       </c>
       <c r="I100">
-        <f t="shared" si="78"/>
+        <f t="shared" si="81"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="J100">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="K100">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>2.5</v>
       </c>
     </row>
@@ -4249,15 +4248,15 @@
         <v>6</v>
       </c>
       <c r="I101">
-        <f t="shared" si="78"/>
+        <f t="shared" si="81"/>
         <v>1.5</v>
       </c>
       <c r="J101">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="K101">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>2.666666666666667</v>
       </c>
     </row>
@@ -4278,15 +4277,15 @@
         <v>8</v>
       </c>
       <c r="I102">
-        <f t="shared" ref="I102" si="81">(2/3)*$B102*((13-E102)/12)</f>
+        <f t="shared" ref="I102" si="84">(2/3)*$B102*((13-E102)/12)</f>
         <v>1.5555555555555556</v>
       </c>
       <c r="J102">
-        <f t="shared" ref="J102" si="82">(2/3)*$B102*((13-F102)/12)</f>
+        <f t="shared" ref="J102" si="85">(2/3)*$B102*((13-F102)/12)</f>
         <v>1.1111111111111112</v>
       </c>
       <c r="K102">
-        <f t="shared" ref="K102" si="83">I102+J102</f>
+        <f t="shared" ref="K102" si="86">I102+J102</f>
         <v>2.666666666666667</v>
       </c>
     </row>
@@ -4336,11 +4335,11 @@
         <v>7</v>
       </c>
       <c r="I105">
-        <f t="shared" ref="I105:J111" si="84">(2/3)*$B105*((13-E105)/12)</f>
+        <f t="shared" ref="I105:J111" si="87">(2/3)*$B105*((13-E105)/12)</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="J105">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>1</v>
       </c>
       <c r="K105">
@@ -4365,11 +4364,11 @@
         <v>3</v>
       </c>
       <c r="I106">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="J106">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="K106">
@@ -4394,11 +4393,11 @@
         <v>3</v>
       </c>
       <c r="I107">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="J107">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="K107">
@@ -4411,29 +4410,29 @@
         <v>111</v>
       </c>
       <c r="I108">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="J108">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="K108">
-        <f t="shared" ref="K108:K111" si="85">I108+J108</f>
+        <f t="shared" ref="K108:K111" si="88">I108+J108</f>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I109">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="J109">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="K109">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
     </row>
@@ -4454,15 +4453,15 @@
         <v>7</v>
       </c>
       <c r="I110">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="J110">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="K110">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>1.4444444444444444</v>
       </c>
     </row>
@@ -4483,15 +4482,15 @@
         <v>2</v>
       </c>
       <c r="I111">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="J111">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0.61111111111111105</v>
       </c>
       <c r="K111">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0.88888888888888884</v>
       </c>
     </row>
@@ -4512,15 +4511,15 @@
         <v>10</v>
       </c>
       <c r="I113">
-        <f t="shared" ref="I113:I115" si="86">(2/3)*$B113*((13-E113)/12)</f>
+        <f t="shared" ref="I113:I115" si="89">(2/3)*$B113*((13-E113)/12)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J113">
-        <f t="shared" ref="J113:J115" si="87">(2/3)*$B113*((13-F113)/12)</f>
+        <f t="shared" ref="J113:J115" si="90">(2/3)*$B113*((13-F113)/12)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="K113">
-        <f t="shared" ref="K113:K115" si="88">I113+J113</f>
+        <f t="shared" ref="K113:K115" si="91">I113+J113</f>
         <v>1</v>
       </c>
     </row>
@@ -4541,15 +4540,15 @@
         <v>5</v>
       </c>
       <c r="I114">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J114">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="K114">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>1.2222222222222221</v>
       </c>
     </row>
@@ -4570,15 +4569,15 @@
         <v>7</v>
       </c>
       <c r="I115">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="J115">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="K115">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>1.2222222222222223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Buffed heavy weapons, fixed points on eldar
</commit_message>
<xml_diff>
--- a/Raw Data/weapons.xlsx
+++ b/Raw Data/weapons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Battlescribe\github\40klite\40klite\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00639559-0EFB-47A7-9141-08D7DD50875A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B8A42F-43B3-4EFE-9E49-6ED23CA538E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{526A3DE0-3542-4F32-9F5D-209F8CA5BDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Heavy" sheetId="1" r:id="rId1"/>
@@ -858,11 +858,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFAFC17-B8CC-4FDE-905B-FC2D8F8BC7C4}">
-  <dimension ref="A1:V115"/>
+  <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +872,7 @@
     <col min="17" max="17" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -919,7 +919,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -975,7 +975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>0.72222222222222221</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I8">
         <f t="shared" ref="I8:I17" si="6">(2/3)*$B8*((13-E8)/12)</f>
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I10">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>1.7777777777777777</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>1.4444444444444444</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1424,8 +1424,12 @@
         <f t="shared" si="8"/>
         <v>1.6666666666666665</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="X15">
+        <f>3.5*5</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2330,26 +2334,26 @@
         <v>-1</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G38">
         <f t="shared" ref="G38:G53" si="31">SUM(D38:F38)/B38</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I38">
         <f t="shared" ref="I38:I53" si="32">(2/3)*$B38*((13-E38)/12)</f>
-        <v>0.44444444444444442</v>
+        <v>0.5</v>
       </c>
       <c r="J38">
         <f t="shared" ref="J38:J53" si="33">(2/3)*$B38*((13-F38)/12)</f>
-        <v>0.16666666666666666</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="K38">
         <f t="shared" ref="K38:K53" si="34">I38+J38</f>
-        <v>0.61111111111111105</v>
+        <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
@@ -2370,11 +2374,11 @@
         <v>5</v>
       </c>
       <c r="F39">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G39">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I39">
         <f t="shared" si="32"/>
@@ -2382,11 +2386,11 @@
       </c>
       <c r="J39">
         <f t="shared" si="33"/>
-        <v>0.27777777777777779</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="K39">
         <f t="shared" si="34"/>
-        <v>0.72222222222222221</v>
+        <v>0.83333333333333326</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -2407,11 +2411,11 @@
         <v>7</v>
       </c>
       <c r="F40">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G40">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I40">
         <f t="shared" si="32"/>
@@ -2419,11 +2423,11 @@
       </c>
       <c r="J40">
         <f t="shared" si="33"/>
-        <v>0.33333333333333331</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="K40">
         <f t="shared" si="34"/>
-        <v>0.66666666666666663</v>
+        <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -2441,18 +2445,18 @@
         <v>-1</v>
       </c>
       <c r="E41">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41">
         <v>4</v>
       </c>
       <c r="G41">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I41">
         <f t="shared" si="32"/>
-        <v>0.16666666666666666</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="J41">
         <f t="shared" si="33"/>
@@ -2460,7 +2464,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="34"/>
-        <v>0.66666666666666663</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="T41" s="2"/>
     </row>
@@ -2479,18 +2483,18 @@
         <v>-2</v>
       </c>
       <c r="E42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42">
         <v>8</v>
       </c>
       <c r="G42">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I42">
         <f t="shared" si="32"/>
-        <v>0.33333333333333331</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J42">
         <f t="shared" si="33"/>
@@ -2498,7 +2502,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="34"/>
-        <v>0.61111111111111116</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -2571,26 +2575,26 @@
         <v>-1</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F45">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G45">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I45">
         <f t="shared" si="32"/>
-        <v>0.44444444444444442</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J45">
         <f t="shared" si="33"/>
-        <v>0.22222222222222221</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K45">
         <f t="shared" si="34"/>
-        <v>0.66666666666666663</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="M45">
         <f>13-((3/5)*(2/3))*12</f>
@@ -2616,18 +2620,18 @@
         <v>-1</v>
       </c>
       <c r="E46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46">
         <v>8</v>
       </c>
       <c r="G46">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I46">
         <f t="shared" si="32"/>
-        <v>0.3888888888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J46">
         <f t="shared" si="33"/>
@@ -2635,7 +2639,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="34"/>
-        <v>0.66666666666666674</v>
+        <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
@@ -2656,11 +2660,11 @@
         <v>5</v>
       </c>
       <c r="F47">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G47">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I47">
         <f t="shared" si="32"/>
@@ -2668,11 +2672,11 @@
       </c>
       <c r="J47">
         <f t="shared" si="33"/>
-        <v>0.27777777777777779</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K47">
         <f t="shared" si="34"/>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777768</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -2690,18 +2694,18 @@
         <v>-2</v>
       </c>
       <c r="E48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48">
         <v>8</v>
       </c>
       <c r="G48">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I48">
         <f t="shared" si="32"/>
-        <v>0.33333333333333331</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J48">
         <f t="shared" si="33"/>
@@ -2709,7 +2713,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="34"/>
-        <v>0.61111111111111116</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -2730,11 +2734,11 @@
         <v>8</v>
       </c>
       <c r="F49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G49">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I49">
         <f t="shared" si="32"/>
@@ -2742,11 +2746,11 @@
       </c>
       <c r="J49">
         <f t="shared" si="33"/>
-        <v>0.33333333333333331</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="K49">
         <f t="shared" si="34"/>
-        <v>0.61111111111111116</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -2767,11 +2771,11 @@
         <v>9</v>
       </c>
       <c r="F50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G50">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I50">
         <f t="shared" si="32"/>
@@ -2779,11 +2783,11 @@
       </c>
       <c r="J50">
         <f t="shared" si="33"/>
-        <v>0.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="K50">
         <f t="shared" si="34"/>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -2801,18 +2805,18 @@
         <v>-1</v>
       </c>
       <c r="E51">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51">
         <v>7</v>
       </c>
       <c r="G51">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I51">
         <f t="shared" si="32"/>
-        <v>0.33333333333333331</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J51">
         <f t="shared" si="33"/>
@@ -2820,7 +2824,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="34"/>
-        <v>0.66666666666666663</v>
+        <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -2841,11 +2845,11 @@
         <v>10</v>
       </c>
       <c r="F52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G52">
         <f t="shared" si="31"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I52">
         <f t="shared" si="32"/>
@@ -2853,11 +2857,11 @@
       </c>
       <c r="J52">
         <f t="shared" si="33"/>
-        <v>0.44444444444444442</v>
+        <v>0.5</v>
       </c>
       <c r="K52">
         <f t="shared" si="34"/>
-        <v>0.61111111111111105</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M52">
         <f>(13-5)/12</f>
@@ -2879,21 +2883,21 @@
         <v>1</v>
       </c>
       <c r="E53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53">
         <v>8</v>
       </c>
       <c r="G53">
         <f t="shared" si="31"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H53" t="s">
         <v>22</v>
       </c>
       <c r="I53">
         <f t="shared" si="32"/>
-        <v>0.44444444444444442</v>
+        <v>0.5</v>
       </c>
       <c r="J53">
         <f t="shared" si="33"/>
@@ -2901,7 +2905,7 @@
       </c>
       <c r="K53">
         <f t="shared" si="34"/>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -2922,11 +2926,11 @@
         <v>8</v>
       </c>
       <c r="F55">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G55">
         <f t="shared" ref="G55:G61" si="37">SUM(D55:F55)/B55</f>
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="I55">
         <f t="shared" ref="I55:J63" si="38">(2/3)*$B55*((13-E55)/12)</f>
@@ -2934,11 +2938,11 @@
       </c>
       <c r="J55">
         <f t="shared" si="38"/>
-        <v>0.66666666666666663</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="K55">
         <f t="shared" ref="K55:K63" si="39">I55+J55</f>
-        <v>1.2222222222222223</v>
+        <v>1.3333333333333335</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -2956,18 +2960,18 @@
         <v>-2</v>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56">
         <v>8</v>
       </c>
       <c r="G56">
         <f t="shared" si="37"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I56">
         <f t="shared" si="38"/>
-        <v>0.33333333333333331</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J56">
         <f t="shared" si="38"/>
@@ -2975,7 +2979,7 @@
       </c>
       <c r="K56">
         <f t="shared" si="39"/>
-        <v>0.61111111111111116</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -2996,11 +3000,11 @@
         <v>5</v>
       </c>
       <c r="F57">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G57">
         <f t="shared" si="37"/>
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="I57">
         <f t="shared" si="38"/>
@@ -3008,11 +3012,11 @@
       </c>
       <c r="J57">
         <f t="shared" si="38"/>
-        <v>0.55555555555555558</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K57">
         <f t="shared" si="39"/>
-        <v>1.4444444444444444</v>
+        <v>1.5555555555555554</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -3144,11 +3148,11 @@
         <v>10</v>
       </c>
       <c r="F61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G61">
         <f t="shared" si="37"/>
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="I61">
         <f t="shared" si="38"/>
@@ -3156,11 +3160,11 @@
       </c>
       <c r="J61">
         <f t="shared" si="38"/>
-        <v>0.88888888888888884</v>
+        <v>1</v>
       </c>
       <c r="K61">
         <f t="shared" si="39"/>
-        <v>1.2222222222222221</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="O61">
         <f>2/3*4</f>
@@ -3185,11 +3189,11 @@
         <v>5</v>
       </c>
       <c r="F62">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G62">
         <f t="shared" ref="G62:G66" si="40">SUM(D62:F62)/B62</f>
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="H62" t="s">
         <v>22</v>
@@ -3200,11 +3204,11 @@
       </c>
       <c r="J62">
         <f t="shared" si="38"/>
-        <v>0.55555555555555558</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K62">
         <f t="shared" si="39"/>
-        <v>1.4444444444444444</v>
+        <v>1.5555555555555554</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>